<commit_message>
Update mục tiêu môn học
</commit_message>
<xml_diff>
--- a/So sanh CTTĐ.xlsx
+++ b/So sanh CTTĐ.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21864" windowHeight="11040" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21864" windowHeight="11040" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CGKL" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="CNOT" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="CNTT" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="ĐCN" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="ĐTCN" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="ĐTCN" sheetId="5" r:id="rId5"/>
     <sheet name="ĐTCN (2)" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet name="ĐTCN (3)" sheetId="9" r:id="rId7"/>
     <sheet name="Điện tử nâng cao" sheetId="10" r:id="rId8"/>
-    <sheet name="Điện kỹ thuật" sheetId="7" r:id="rId9"/>
-    <sheet name="đo lường điện tử" sheetId="8" r:id="rId10"/>
+    <sheet name="CheTaoMachIn" sheetId="11" r:id="rId9"/>
+    <sheet name="LichTrinhCacMon" sheetId="12" r:id="rId10"/>
+    <sheet name="Điện kỹ thuật" sheetId="7" r:id="rId11"/>
+    <sheet name="đo lường điện tử" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -178,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="476">
   <si>
     <t>SO SÁNH CHƯƠNG TRÌNH ĐÀO TẠO NGHỀ CẮT GỌT KIM LOẠI</t>
   </si>
@@ -1578,6 +1580,68 @@
   </si>
   <si>
     <t>2.5. Bài tập ứng dụng</t>
+  </si>
+  <si>
+    <t>Phần I: Kỹ thuật hàn mạch in</t>
+  </si>
+  <si>
+    <t>Bài 1 : Thao tác đảm bảo an toàn vị trí hàn và kỹ thuật sử dụng các dụng cụ hàn</t>
+  </si>
+  <si>
+    <t>Phần II: Thiết kế và chế tạo mạch in</t>
+  </si>
+  <si>
+    <t>Bài 2: Chế tạo mạch in thủ công</t>
+  </si>
+  <si>
+    <t>Bài 3: Kiểm tra mạch sau chế tạo</t>
+  </si>
+  <si>
+    <t>Bài 4: Đồ án môn học</t>
+  </si>
+  <si>
+    <t>Cộng</t>
+  </si>
+  <si>
+    <t>Bài 2 : Kỹ thuật hàn nối dây, hàn linh kiện xuyên lỗ, xử lý mạch sau hàn và tháo mối hàn linh kiện xuyên lỗ.</t>
+  </si>
+  <si>
+    <t>Bài 1: Quy trình sản xuất sản phẩm điện tử và chế tạo mạch in</t>
+  </si>
+  <si>
+    <t>Thứ tự bài giảng</t>
+  </si>
+  <si>
+    <t>Tên bài giảng</t>
+  </si>
+  <si>
+    <t>Thời lượng thực hiện</t>
+  </si>
+  <si>
+    <t>Thiết bị, phương tiện, đồ dùng dạy học</t>
+  </si>
+  <si>
+    <t>Lớp: ĐI.1.02A</t>
+  </si>
+  <si>
+    <t>Lớp: ĐI.1.02B</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Giáo án, đề cương bài giảng, vật tư, máy tính</t>
+  </si>
+  <si>
+    <t>Bài 1: Thao tác đảm bảo an toàn vị trí hàn và kỹ thuật sử dụng các dụng cụ hàn</t>
+  </si>
+  <si>
+    <t>Bài 2: Kỹ thuật hàn nối dây, hàn linh kiện xuyên lỗ, xử lý mạch sau hàn và tháo mối hàn linh kiện xuyên lỗ.</t>
+  </si>
+  <si>
+    <t>Bài 3: Kiểm tra mạch sau chế tạo
+Kiểm tra lý thuyết 1 tiết
+Kiểm tra thực hành 1 tiết</t>
   </si>
 </sst>
 </file>
@@ -1937,7 +2001,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -2192,6 +2256,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2206,7 +2279,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2694,6 +2767,62 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2748,6 +2877,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2761,6 +2896,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2787,13 +2928,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2806,13 +2941,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2828,29 +2963,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3187,59 +3299,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
+      <c r="A2" s="225" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="226" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201" t="s">
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="201"/>
-      <c r="J3" s="201"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="202" t="s">
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="201" t="s">
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="227" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="200"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -3282,7 +3394,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="201"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -3315,10 +3427,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="218" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="193"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -3653,10 +3765,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="194" t="s">
+      <c r="B13" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="195"/>
+      <c r="C13" s="221"/>
       <c r="D13" s="18">
         <f>+D14+D27</f>
         <v>2355</v>
@@ -3679,10 +3791,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8"/>
-      <c r="B14" s="196" t="s">
+      <c r="B14" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="197"/>
+      <c r="C14" s="223"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D26)</f>
         <v>570</v>
@@ -4320,10 +4432,10 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="8"/>
-      <c r="B27" s="198" t="s">
+      <c r="B27" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="198"/>
+      <c r="C27" s="224"/>
       <c r="D27" s="22">
         <f>+SUM(D28:D50)</f>
         <v>1785</v>
@@ -4584,23 +4696,23 @@
       <c r="K32" s="14">
         <v>3</v>
       </c>
-      <c r="L32" s="189">
+      <c r="L32" s="215">
         <f>+H32+H33+H34-D32-D33-D34-D35-D39-D41-D42-D43-D52-D53</f>
         <v>-365</v>
       </c>
-      <c r="M32" s="189">
+      <c r="M32" s="215">
         <f t="shared" ref="M32:O32" si="7">+I32+I33+I34-E32-E33-E34-E35-E39-E41-E42-E43-E52-E53</f>
         <v>-77</v>
       </c>
-      <c r="N32" s="189">
+      <c r="N32" s="215">
         <f t="shared" si="7"/>
         <v>-276</v>
       </c>
-      <c r="O32" s="189">
+      <c r="O32" s="215">
         <f t="shared" si="7"/>
         <v>-12</v>
       </c>
-      <c r="P32" s="189" t="s">
+      <c r="P32" s="215" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4638,11 +4750,11 @@
       <c r="K33" s="14">
         <v>3</v>
       </c>
-      <c r="L33" s="190"/>
-      <c r="M33" s="190"/>
-      <c r="N33" s="190"/>
-      <c r="O33" s="190"/>
-      <c r="P33" s="190"/>
+      <c r="L33" s="216"/>
+      <c r="M33" s="216"/>
+      <c r="N33" s="216"/>
+      <c r="O33" s="216"/>
+      <c r="P33" s="216"/>
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="33">
@@ -4678,11 +4790,11 @@
       <c r="K34" s="14">
         <v>4</v>
       </c>
-      <c r="L34" s="191"/>
-      <c r="M34" s="191"/>
-      <c r="N34" s="191"/>
-      <c r="O34" s="191"/>
-      <c r="P34" s="191"/>
+      <c r="L34" s="217"/>
+      <c r="M34" s="217"/>
+      <c r="N34" s="217"/>
+      <c r="O34" s="217"/>
+      <c r="P34" s="217"/>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="33">
@@ -4718,23 +4830,23 @@
       <c r="K35" s="14">
         <v>3</v>
       </c>
-      <c r="L35" s="189">
+      <c r="L35" s="215">
         <f>+H35+H36-D36-D37-D38-D44-D45-D46-D54-D55-D56-D57-D58</f>
         <v>-500</v>
       </c>
-      <c r="M35" s="189">
+      <c r="M35" s="215">
         <f t="shared" ref="M35:O35" si="8">+I35+I36-E36-E37-E38-E44-E45-E46-E54-E55-E56-E57-E58</f>
         <v>-65</v>
       </c>
-      <c r="N35" s="189">
+      <c r="N35" s="215">
         <f t="shared" si="8"/>
         <v>-422</v>
       </c>
-      <c r="O35" s="189">
+      <c r="O35" s="215">
         <f t="shared" si="8"/>
         <v>-13</v>
       </c>
-      <c r="P35" s="189" t="s">
+      <c r="P35" s="215" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4772,11 +4884,11 @@
       <c r="K36" s="14">
         <v>3</v>
       </c>
-      <c r="L36" s="191"/>
-      <c r="M36" s="191"/>
-      <c r="N36" s="191"/>
-      <c r="O36" s="191"/>
-      <c r="P36" s="191"/>
+      <c r="L36" s="217"/>
+      <c r="M36" s="217"/>
+      <c r="N36" s="217"/>
+      <c r="O36" s="217"/>
+      <c r="P36" s="217"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="33">
@@ -5312,10 +5424,10 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="33"/>
-      <c r="B51" s="187" t="s">
+      <c r="B51" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="188"/>
+      <c r="C51" s="214"/>
       <c r="D51" s="4">
         <f>+SUM(D52:D62)</f>
         <v>945</v>
@@ -5823,9 +5935,841 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="14.4" customHeight="1">
+      <c r="A1" s="193" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="193" t="s">
+        <v>466</v>
+      </c>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="G1" s="193" t="s">
+        <v>467</v>
+      </c>
+      <c r="H1" s="193"/>
+      <c r="I1" s="193"/>
+      <c r="J1" s="193"/>
+      <c r="K1" s="193" t="s">
+        <v>468</v>
+      </c>
+      <c r="L1" s="193" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="195"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193" t="s">
+        <v>469</v>
+      </c>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193" t="s">
+        <v>470</v>
+      </c>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="197"/>
+      <c r="C3" s="193" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" s="193" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="193" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="193" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="193" t="s">
+        <v>471</v>
+      </c>
+      <c r="H3" s="193" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="193" t="s">
+        <v>471</v>
+      </c>
+      <c r="J3" s="193" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="43.2">
+      <c r="A4" s="253">
+        <v>1</v>
+      </c>
+      <c r="B4" s="200" t="s">
+        <v>473</v>
+      </c>
+      <c r="C4" s="201">
+        <f>SUM(D4:E4)</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="201">
+        <v>1</v>
+      </c>
+      <c r="E4" s="201">
+        <v>1</v>
+      </c>
+      <c r="F4" s="201"/>
+      <c r="G4" s="201"/>
+      <c r="H4" s="201"/>
+      <c r="I4" s="201"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202" t="s">
+        <v>472</v>
+      </c>
+      <c r="L4" s="203"/>
+    </row>
+    <row r="5" spans="1:12" ht="57.6">
+      <c r="A5" s="254"/>
+      <c r="B5" s="204" t="s">
+        <v>474</v>
+      </c>
+      <c r="C5" s="205">
+        <f t="shared" ref="C5:C9" si="0">SUM(D5:E5)</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="205">
+        <v>1</v>
+      </c>
+      <c r="E5" s="205">
+        <v>3</v>
+      </c>
+      <c r="F5" s="205"/>
+      <c r="G5" s="205"/>
+      <c r="H5" s="205"/>
+      <c r="I5" s="205"/>
+      <c r="J5" s="206"/>
+      <c r="K5" s="206"/>
+      <c r="L5" s="207"/>
+    </row>
+    <row r="6" spans="1:12" ht="43.2">
+      <c r="A6" s="253">
+        <v>2</v>
+      </c>
+      <c r="B6" s="200" t="s">
+        <v>464</v>
+      </c>
+      <c r="C6" s="201">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="201">
+        <v>4</v>
+      </c>
+      <c r="E6" s="201">
+        <v>0</v>
+      </c>
+      <c r="F6" s="201"/>
+      <c r="G6" s="201"/>
+      <c r="H6" s="201"/>
+      <c r="I6" s="201"/>
+      <c r="J6" s="202"/>
+      <c r="K6" s="202"/>
+      <c r="L6" s="203"/>
+    </row>
+    <row r="7" spans="1:12" ht="31.2" customHeight="1">
+      <c r="A7" s="254"/>
+      <c r="B7" s="204" t="s">
+        <v>459</v>
+      </c>
+      <c r="C7" s="205">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D7" s="205">
+        <v>0</v>
+      </c>
+      <c r="E7" s="205">
+        <v>2</v>
+      </c>
+      <c r="F7" s="205"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="205"/>
+      <c r="I7" s="205"/>
+      <c r="J7" s="206"/>
+      <c r="K7" s="206" t="s">
+        <v>472</v>
+      </c>
+      <c r="L7" s="207"/>
+    </row>
+    <row r="8" spans="1:12" ht="29.4" customHeight="1">
+      <c r="A8" s="208">
+        <v>3</v>
+      </c>
+      <c r="B8" s="209" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8" s="210">
+        <f>SUM(D8:F8)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="210">
+        <v>0</v>
+      </c>
+      <c r="E8" s="210">
+        <v>6</v>
+      </c>
+      <c r="F8" s="210"/>
+      <c r="G8" s="210"/>
+      <c r="H8" s="210"/>
+      <c r="I8" s="210"/>
+      <c r="J8" s="211"/>
+      <c r="K8" s="211"/>
+      <c r="L8" s="212"/>
+    </row>
+    <row r="9" spans="1:12" ht="57.6">
+      <c r="A9" s="208">
+        <v>4</v>
+      </c>
+      <c r="B9" s="209" t="s">
+        <v>475</v>
+      </c>
+      <c r="C9" s="210">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="210">
+        <v>0</v>
+      </c>
+      <c r="E9" s="210">
+        <v>4</v>
+      </c>
+      <c r="F9" s="210">
+        <v>2</v>
+      </c>
+      <c r="G9" s="210"/>
+      <c r="H9" s="210"/>
+      <c r="I9" s="210"/>
+      <c r="J9" s="211"/>
+      <c r="K9" s="211"/>
+      <c r="L9" s="212"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="199"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="199"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="199"/>
+      <c r="G10" s="199"/>
+      <c r="H10" s="199"/>
+      <c r="I10" s="199"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="199"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="199"/>
+      <c r="E11" s="199"/>
+      <c r="F11" s="199"/>
+      <c r="G11" s="199"/>
+      <c r="H11" s="199"/>
+      <c r="I11" s="199"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="199"/>
+      <c r="C12" s="199"/>
+      <c r="D12" s="199"/>
+      <c r="E12" s="199"/>
+      <c r="F12" s="199"/>
+      <c r="G12" s="199"/>
+      <c r="H12" s="199"/>
+      <c r="I12" s="199"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="199"/>
+      <c r="C13" s="199"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="199"/>
+      <c r="G13" s="199"/>
+      <c r="H13" s="199"/>
+      <c r="I13" s="199"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="199"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="199"/>
+      <c r="I14" s="199"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="199"/>
+      <c r="C15" s="199"/>
+      <c r="D15" s="199"/>
+      <c r="E15" s="199"/>
+      <c r="F15" s="199"/>
+      <c r="G15" s="199"/>
+      <c r="H15" s="199"/>
+      <c r="I15" s="199"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="199"/>
+      <c r="C16" s="199"/>
+      <c r="D16" s="199"/>
+      <c r="E16" s="199"/>
+      <c r="F16" s="199"/>
+      <c r="G16" s="199"/>
+      <c r="H16" s="199"/>
+      <c r="I16" s="199"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="199"/>
+      <c r="C17" s="199"/>
+      <c r="D17" s="199"/>
+      <c r="E17" s="199"/>
+      <c r="F17" s="199"/>
+      <c r="G17" s="199"/>
+      <c r="H17" s="199"/>
+      <c r="I17" s="199"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="199"/>
+      <c r="C18" s="199"/>
+      <c r="D18" s="199"/>
+      <c r="E18" s="199"/>
+      <c r="F18" s="199"/>
+      <c r="G18" s="199"/>
+      <c r="H18" s="199"/>
+      <c r="I18" s="199"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="199"/>
+      <c r="C19" s="199"/>
+      <c r="D19" s="199"/>
+      <c r="E19" s="199"/>
+      <c r="F19" s="199"/>
+      <c r="G19" s="199"/>
+      <c r="H19" s="199"/>
+      <c r="I19" s="199"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="199"/>
+      <c r="C20" s="199"/>
+      <c r="D20" s="199"/>
+      <c r="E20" s="199"/>
+      <c r="F20" s="199"/>
+      <c r="G20" s="199"/>
+      <c r="H20" s="199"/>
+      <c r="I20" s="199"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="199"/>
+      <c r="C21" s="199"/>
+      <c r="D21" s="199"/>
+      <c r="E21" s="199"/>
+      <c r="F21" s="199"/>
+      <c r="G21" s="199"/>
+      <c r="H21" s="199"/>
+      <c r="I21" s="199"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="199"/>
+      <c r="C22" s="199"/>
+      <c r="D22" s="199"/>
+      <c r="E22" s="199"/>
+      <c r="F22" s="199"/>
+      <c r="G22" s="199"/>
+      <c r="H22" s="199"/>
+      <c r="I22" s="199"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="199"/>
+      <c r="C23" s="199"/>
+      <c r="D23" s="199"/>
+      <c r="E23" s="199"/>
+      <c r="F23" s="199"/>
+      <c r="G23" s="199"/>
+      <c r="H23" s="199"/>
+      <c r="I23" s="199"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A1" s="255" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="255" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="257" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
+      <c r="F1" s="259"/>
+    </row>
+    <row r="2" spans="1:6" ht="51" thickBot="1">
+      <c r="A2" s="256"/>
+      <c r="B2" s="256"/>
+      <c r="C2" s="107" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" s="107" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="107" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" s="107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A3" s="108" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="109" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="107">
+        <f>SUM(D3:F3)</f>
+        <v>5</v>
+      </c>
+      <c r="D3" s="107">
+        <f>SUM(D4:D7)</f>
+        <v>4</v>
+      </c>
+      <c r="E3" s="107">
+        <f t="shared" ref="E3" si="0">SUM(E4:E7)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="107"/>
+    </row>
+    <row r="4" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A4" s="111">
+        <v>1</v>
+      </c>
+      <c r="B4" s="112" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="113"/>
+      <c r="D4" s="114">
+        <v>1</v>
+      </c>
+      <c r="E4" s="113"/>
+      <c r="F4" s="110"/>
+    </row>
+    <row r="5" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A5" s="111">
+        <v>2</v>
+      </c>
+      <c r="B5" s="112" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="113"/>
+      <c r="D5" s="114">
+        <v>1</v>
+      </c>
+      <c r="E5" s="113"/>
+      <c r="F5" s="110"/>
+    </row>
+    <row r="6" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A6" s="111">
+        <v>3</v>
+      </c>
+      <c r="B6" s="112" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="113"/>
+      <c r="D6" s="114">
+        <v>1</v>
+      </c>
+      <c r="E6" s="113"/>
+      <c r="F6" s="110"/>
+    </row>
+    <row r="7" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A7" s="111">
+        <v>4</v>
+      </c>
+      <c r="B7" s="112" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="113"/>
+      <c r="D7" s="114">
+        <v>1</v>
+      </c>
+      <c r="E7" s="114">
+        <v>1</v>
+      </c>
+      <c r="F7" s="110"/>
+    </row>
+    <row r="8" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A8" s="108" t="s">
+        <v>317</v>
+      </c>
+      <c r="B8" s="109" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="107">
+        <f>SUM(D8:F8)</f>
+        <v>16</v>
+      </c>
+      <c r="D8" s="107">
+        <f>SUM(D9:D11)</f>
+        <v>9</v>
+      </c>
+      <c r="E8" s="107">
+        <f t="shared" ref="E8" si="1">SUM(E9:E11)</f>
+        <v>6</v>
+      </c>
+      <c r="F8" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34.200000000000003" thickBot="1">
+      <c r="A9" s="111">
+        <v>1</v>
+      </c>
+      <c r="B9" s="112" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="113"/>
+      <c r="D9" s="114">
+        <v>1</v>
+      </c>
+      <c r="E9" s="114">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="110"/>
+    </row>
+    <row r="10" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A10" s="111">
+        <v>2</v>
+      </c>
+      <c r="B10" s="112" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="113"/>
+      <c r="D10" s="114">
+        <v>1</v>
+      </c>
+      <c r="E10" s="114">
+        <v>1</v>
+      </c>
+      <c r="F10" s="110"/>
+    </row>
+    <row r="11" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A11" s="111">
+        <v>3</v>
+      </c>
+      <c r="B11" s="112" t="s">
+        <v>321</v>
+      </c>
+      <c r="C11" s="113"/>
+      <c r="D11" s="114">
+        <v>7</v>
+      </c>
+      <c r="E11" s="114">
+        <v>4.5</v>
+      </c>
+      <c r="F11" s="110"/>
+    </row>
+    <row r="12" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A12" s="108" t="s">
+        <v>322</v>
+      </c>
+      <c r="B12" s="109" t="s">
+        <v>323</v>
+      </c>
+      <c r="C12" s="107">
+        <f>SUM(D12:F12)</f>
+        <v>17</v>
+      </c>
+      <c r="D12" s="107">
+        <f>SUM(D13:D16)</f>
+        <v>11</v>
+      </c>
+      <c r="E12" s="107">
+        <f t="shared" ref="E12" si="2">SUM(E13:E16)</f>
+        <v>5</v>
+      </c>
+      <c r="F12" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A13" s="111">
+        <v>1</v>
+      </c>
+      <c r="B13" s="112" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="113"/>
+      <c r="D13" s="114">
+        <v>1</v>
+      </c>
+      <c r="E13" s="114">
+        <v>1</v>
+      </c>
+      <c r="F13" s="110"/>
+    </row>
+    <row r="14" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A14" s="111">
+        <v>2</v>
+      </c>
+      <c r="B14" s="112" t="s">
+        <v>325</v>
+      </c>
+      <c r="C14" s="113"/>
+      <c r="D14" s="114">
+        <v>3</v>
+      </c>
+      <c r="E14" s="114">
+        <v>1</v>
+      </c>
+      <c r="F14" s="110"/>
+    </row>
+    <row r="15" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A15" s="111">
+        <v>3</v>
+      </c>
+      <c r="B15" s="112" t="s">
+        <v>326</v>
+      </c>
+      <c r="C15" s="113"/>
+      <c r="D15" s="114">
+        <v>3</v>
+      </c>
+      <c r="E15" s="114">
+        <v>1</v>
+      </c>
+      <c r="F15" s="110"/>
+    </row>
+    <row r="16" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A16" s="111">
+        <v>4</v>
+      </c>
+      <c r="B16" s="112" t="s">
+        <v>327</v>
+      </c>
+      <c r="C16" s="113"/>
+      <c r="D16" s="114">
+        <v>4</v>
+      </c>
+      <c r="E16" s="114">
+        <v>2</v>
+      </c>
+      <c r="F16" s="110"/>
+    </row>
+    <row r="17" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A17" s="108" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="109" t="s">
+        <v>329</v>
+      </c>
+      <c r="C17" s="107">
+        <f>SUM(D17:F17)</f>
+        <v>17</v>
+      </c>
+      <c r="D17" s="107">
+        <f>SUM(D18:D20)</f>
+        <v>10</v>
+      </c>
+      <c r="E17" s="107">
+        <f>SUM(E18:E20)</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A18" s="111">
+        <v>1</v>
+      </c>
+      <c r="B18" s="112" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" s="113"/>
+      <c r="D18" s="114">
+        <v>4</v>
+      </c>
+      <c r="E18" s="114">
+        <v>3</v>
+      </c>
+      <c r="F18" s="110"/>
+    </row>
+    <row r="19" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A19" s="111">
+        <v>3</v>
+      </c>
+      <c r="B19" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="C19" s="113"/>
+      <c r="D19" s="114">
+        <v>3</v>
+      </c>
+      <c r="E19" s="114">
+        <v>1</v>
+      </c>
+      <c r="F19" s="110"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A20" s="111">
+        <v>4</v>
+      </c>
+      <c r="B20" s="112" t="s">
+        <v>332</v>
+      </c>
+      <c r="C20" s="113"/>
+      <c r="D20" s="114">
+        <v>3</v>
+      </c>
+      <c r="E20" s="114">
+        <v>2</v>
+      </c>
+      <c r="F20" s="110"/>
+    </row>
+    <row r="21" spans="1:6" ht="34.200000000000003" thickBot="1">
+      <c r="A21" s="108" t="s">
+        <v>333</v>
+      </c>
+      <c r="B21" s="109" t="s">
+        <v>334</v>
+      </c>
+      <c r="C21" s="107">
+        <f>SUM(D21:F21)</f>
+        <v>5</v>
+      </c>
+      <c r="D21" s="107">
+        <f>SUM(D22:D23)</f>
+        <v>2</v>
+      </c>
+      <c r="E21" s="107">
+        <f>SUM(E22:E23)</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A22" s="111">
+        <v>1</v>
+      </c>
+      <c r="B22" s="112" t="s">
+        <v>335</v>
+      </c>
+      <c r="C22" s="113"/>
+      <c r="D22" s="114">
+        <v>1</v>
+      </c>
+      <c r="E22" s="114">
+        <v>1</v>
+      </c>
+      <c r="F22" s="110"/>
+    </row>
+    <row r="23" spans="1:6" ht="34.200000000000003" thickBot="1">
+      <c r="A23" s="111">
+        <v>2</v>
+      </c>
+      <c r="B23" s="112" t="s">
+        <v>336</v>
+      </c>
+      <c r="C23" s="113"/>
+      <c r="D23" s="114">
+        <v>1</v>
+      </c>
+      <c r="E23" s="114">
+        <v>1</v>
+      </c>
+      <c r="F23" s="110"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.399999999999999" thickBot="1">
+      <c r="A24" s="257" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="259"/>
+      <c r="C24" s="107">
+        <f>SUM(C3,C8,C12,C17,C21)</f>
+        <v>60</v>
+      </c>
+      <c r="D24" s="107">
+        <f>SUM(D3,D8,D12,D17,D21)</f>
+        <v>36</v>
+      </c>
+      <c r="E24" s="107">
+        <f>SUM(E3,E8,E12,E17,E21)</f>
+        <v>20</v>
+      </c>
+      <c r="F24" s="107">
+        <f>SUM(F3,F8,F12,F17,F21)</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A24:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -5836,20 +6780,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999">
-      <c r="A1" s="225"/>
-      <c r="B1" s="225" t="s">
+      <c r="A1" s="252"/>
+      <c r="B1" s="252" t="s">
         <v>337</v>
       </c>
-      <c r="C1" s="225" t="s">
+      <c r="C1" s="252" t="s">
         <v>308</v>
       </c>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
     </row>
     <row r="2" spans="1:6" ht="69.599999999999994">
-      <c r="A2" s="225"/>
-      <c r="B2" s="225"/>
+      <c r="A2" s="252"/>
+      <c r="B2" s="252"/>
       <c r="C2" s="116" t="s">
         <v>309</v>
       </c>
@@ -6440,59 +7384,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="225" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="226" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201" t="s">
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="201"/>
-      <c r="J3" s="201"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="202" t="s">
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="201" t="s">
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="227" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="200"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -6535,7 +7479,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="201"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -6568,10 +7512,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="218" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="193"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -6906,10 +7850,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="194" t="s">
+      <c r="B13" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="195"/>
+      <c r="C13" s="221"/>
       <c r="D13" s="18">
         <f>+D14+D29</f>
         <v>2475</v>
@@ -6932,10 +7876,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8"/>
-      <c r="B14" s="196" t="s">
+      <c r="B14" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="197"/>
+      <c r="C14" s="223"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D28)</f>
         <v>645</v>
@@ -7661,10 +8605,10 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="8"/>
-      <c r="B29" s="198" t="s">
+      <c r="B29" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="198"/>
+      <c r="C29" s="224"/>
       <c r="D29" s="22">
         <f>+SUM(D30:D46)</f>
         <v>1830</v>
@@ -8539,10 +9483,10 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="33"/>
-      <c r="B47" s="187" t="s">
+      <c r="B47" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="188"/>
+      <c r="C47" s="214"/>
       <c r="D47" s="4">
         <f>+SUM(D48:D55)</f>
         <v>855</v>
@@ -9032,59 +9976,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="17.399999999999999">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="225" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
       <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="226" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201" t="s">
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="201"/>
-      <c r="J3" s="201"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="202" t="s">
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="201" t="s">
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="227" t="s">
         <v>5</v>
       </c>
       <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" ht="27.6">
-      <c r="A4" s="200"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -9127,7 +10071,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="201"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="4"/>
@@ -9159,10 +10103,10 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="4"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="218" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="193"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -9497,10 +10441,10 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="21"/>
-      <c r="B13" s="194" t="s">
+      <c r="B13" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="195"/>
+      <c r="C13" s="221"/>
       <c r="D13" s="18">
         <f>+D14+D26</f>
         <v>3325</v>
@@ -9523,10 +10467,10 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="8"/>
-      <c r="B14" s="196" t="s">
+      <c r="B14" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="197"/>
+      <c r="C14" s="223"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D25)</f>
         <v>660</v>
@@ -10091,10 +11035,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="8"/>
-      <c r="B26" s="198" t="s">
+      <c r="B26" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="198"/>
+      <c r="C26" s="224"/>
       <c r="D26" s="22">
         <f>+SUM(D27:D49)</f>
         <v>2665</v>
@@ -11085,10 +12029,10 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="33"/>
-      <c r="B50" s="187" t="s">
+      <c r="B50" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="188"/>
+      <c r="C50" s="214"/>
       <c r="D50" s="4">
         <f>+SUM(D51:D61)</f>
         <v>900</v>
@@ -11767,59 +12711,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="225" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="226" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201" t="s">
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="201"/>
-      <c r="J3" s="201"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="202" t="s">
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="201" t="s">
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="227" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="200"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -11862,7 +12806,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="201"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -11895,10 +12839,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="218" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="193"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -12233,10 +13177,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="194" t="s">
+      <c r="B13" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="195"/>
+      <c r="C13" s="221"/>
       <c r="D13" s="18">
         <f>+D14+D33</f>
         <v>2520</v>
@@ -12259,10 +13203,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8"/>
-      <c r="B14" s="196" t="s">
+      <c r="B14" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="197"/>
+      <c r="C14" s="223"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D32)</f>
         <v>445</v>
@@ -13009,10 +13953,10 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="8"/>
-      <c r="B33" s="198" t="s">
+      <c r="B33" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="198"/>
+      <c r="C33" s="224"/>
       <c r="D33" s="22">
         <f>+SUM(D34:D50)</f>
         <v>2075</v>
@@ -13673,10 +14617,10 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="33"/>
-      <c r="B51" s="187" t="s">
+      <c r="B51" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="188"/>
+      <c r="C51" s="214"/>
       <c r="D51" s="4">
         <f>+SUM(D52:D58)</f>
         <v>780</v>
@@ -14022,7 +14966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AE54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -14045,59 +14989,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="225" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="226" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201" t="s">
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="201"/>
-      <c r="J3" s="201"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="202" t="s">
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="201" t="s">
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="227" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="200"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -14140,7 +15084,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="201"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -14173,10 +15117,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="218" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="193"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -14511,8 +15455,8 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="203"/>
-      <c r="C13" s="204"/>
+      <c r="B13" s="229"/>
+      <c r="C13" s="230"/>
       <c r="D13" s="18"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -14529,10 +15473,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="21"/>
-      <c r="B14" s="194" t="s">
+      <c r="B14" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="195"/>
+      <c r="C14" s="221"/>
       <c r="D14" s="18">
         <f>+D15+D26</f>
         <v>2460</v>
@@ -14555,10 +15499,10 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="8"/>
-      <c r="B15" s="196" t="s">
+      <c r="B15" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="197"/>
+      <c r="C15" s="223"/>
       <c r="D15" s="22">
         <f>+SUM(D16:D25)</f>
         <v>810</v>
@@ -15101,10 +16045,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="8"/>
-      <c r="B26" s="198" t="s">
+      <c r="B26" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="198"/>
+      <c r="C26" s="224"/>
       <c r="D26" s="22">
         <f>+SUM(D27:D39)</f>
         <v>1650</v>
@@ -15793,10 +16737,10 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="33"/>
-      <c r="B40" s="187" t="s">
+      <c r="B40" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="188"/>
+      <c r="C40" s="214"/>
       <c r="D40" s="4">
         <f>+SUM(D41:D51)</f>
         <v>1230</v>
@@ -16430,59 +17374,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="23.25" customHeight="1">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="225" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
+      <c r="B2" s="225"/>
+      <c r="C2" s="225"/>
+      <c r="D2" s="225"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="225"/>
+      <c r="G2" s="225"/>
+      <c r="H2" s="225"/>
+      <c r="I2" s="225"/>
+      <c r="J2" s="225"/>
+      <c r="K2" s="225"/>
+      <c r="L2" s="225"/>
+      <c r="M2" s="225"/>
+      <c r="N2" s="225"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="226" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="226" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200" t="s">
+      <c r="C3" s="226"/>
+      <c r="D3" s="226" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201" t="s">
+      <c r="E3" s="226"/>
+      <c r="F3" s="226"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="201"/>
-      <c r="J3" s="201"/>
-      <c r="K3" s="201"/>
-      <c r="L3" s="202" t="s">
+      <c r="I3" s="227"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="227"/>
+      <c r="L3" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="201" t="s">
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
+      <c r="P3" s="227" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="200"/>
+      <c r="A4" s="226"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -16525,7 +17469,7 @@
       <c r="O4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="201"/>
+      <c r="P4" s="227"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="84"/>
@@ -16558,10 +17502,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="84"/>
-      <c r="B6" s="192" t="s">
+      <c r="B6" s="218" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="193"/>
+      <c r="C6" s="219"/>
       <c r="D6" s="85">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -16902,8 +17846,8 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="203"/>
-      <c r="C13" s="204"/>
+      <c r="B13" s="229"/>
+      <c r="C13" s="230"/>
       <c r="D13" s="18"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -16920,10 +17864,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="21"/>
-      <c r="B14" s="194" t="s">
+      <c r="B14" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="195"/>
+      <c r="C14" s="221"/>
       <c r="D14" s="18">
         <f>+D15+D26</f>
         <v>2510</v>
@@ -16946,10 +17890,10 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="8"/>
-      <c r="B15" s="196" t="s">
+      <c r="B15" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="197"/>
+      <c r="C15" s="223"/>
       <c r="D15" s="22">
         <f>+SUM(D16:D25)</f>
         <v>860</v>
@@ -17502,10 +18446,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="8"/>
-      <c r="B26" s="198" t="s">
+      <c r="B26" s="224" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="198"/>
+      <c r="C26" s="224"/>
       <c r="D26" s="22">
         <f>+SUM(D27:D38)</f>
         <v>1650</v>
@@ -18164,10 +19108,10 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="33"/>
-      <c r="B39" s="187" t="s">
+      <c r="B39" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="188"/>
+      <c r="C39" s="214"/>
       <c r="D39" s="84">
         <f>+SUM(D41:D48)</f>
         <v>787</v>
@@ -18596,8 +19540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.25" customHeight="1"/>
@@ -18621,86 +19565,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="34.5" customHeight="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="237" t="s">
         <v>417</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
+      <c r="B1" s="237"/>
+      <c r="C1" s="237"/>
+      <c r="D1" s="237"/>
+      <c r="E1" s="237"/>
+      <c r="F1" s="237"/>
+      <c r="G1" s="237"/>
     </row>
     <row r="2" spans="1:31" ht="20.25" hidden="1" customHeight="1">
-      <c r="A2" s="224" t="s">
+      <c r="A2" s="231" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="224"/>
-      <c r="C2" s="224"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="224"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="224"/>
-      <c r="H2" s="224"/>
-      <c r="I2" s="224"/>
-      <c r="J2" s="224"/>
-      <c r="K2" s="224"/>
-      <c r="L2" s="224"/>
-      <c r="M2" s="224"/>
-      <c r="N2" s="224"/>
-      <c r="O2" s="224"/>
-      <c r="P2" s="224"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="231"/>
+      <c r="H2" s="231"/>
+      <c r="I2" s="231"/>
+      <c r="J2" s="231"/>
+      <c r="K2" s="231"/>
+      <c r="L2" s="231"/>
+      <c r="M2" s="231"/>
+      <c r="N2" s="231"/>
+      <c r="O2" s="231"/>
+      <c r="P2" s="231"/>
       <c r="AE2" s="146"/>
     </row>
     <row r="3" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A3" s="225" t="s">
+      <c r="A3" s="252" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="212" t="s">
+      <c r="B3" s="242" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="213"/>
-      <c r="D3" s="226" t="s">
+      <c r="C3" s="243"/>
+      <c r="D3" s="239" t="s">
         <v>421</v>
       </c>
-      <c r="E3" s="226"/>
-      <c r="F3" s="226"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="220" t="s">
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="239"/>
+      <c r="H3" s="238" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="226"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="226"/>
-      <c r="L3" s="224" t="s">
+      <c r="I3" s="239"/>
+      <c r="J3" s="239"/>
+      <c r="K3" s="239"/>
+      <c r="L3" s="231" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="224"/>
-      <c r="N3" s="224"/>
-      <c r="O3" s="224"/>
-      <c r="P3" s="218" t="s">
+      <c r="M3" s="231"/>
+      <c r="N3" s="231"/>
+      <c r="O3" s="231"/>
+      <c r="P3" s="232" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="205" t="s">
+      <c r="Q3" s="233" t="s">
         <v>424</v>
       </c>
-      <c r="R3" s="207" t="s">
+      <c r="R3" s="235" t="s">
         <v>427</v>
       </c>
       <c r="AE3" s="146"/>
     </row>
     <row r="4" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A4" s="225"/>
-      <c r="B4" s="214"/>
-      <c r="C4" s="215"/>
-      <c r="D4" s="207" t="s">
+      <c r="A4" s="252"/>
+      <c r="B4" s="244"/>
+      <c r="C4" s="245"/>
+      <c r="D4" s="235" t="s">
         <v>420</v>
       </c>
-      <c r="E4" s="218" t="s">
+      <c r="E4" s="232" t="s">
         <v>422</v>
       </c>
-      <c r="F4" s="219"/>
-      <c r="G4" s="220"/>
+      <c r="F4" s="248"/>
+      <c r="G4" s="238"/>
       <c r="H4" s="167"/>
       <c r="I4" s="132"/>
       <c r="J4" s="132"/>
@@ -18709,16 +19653,16 @@
       <c r="M4" s="134"/>
       <c r="N4" s="134"/>
       <c r="O4" s="134"/>
-      <c r="P4" s="218"/>
-      <c r="Q4" s="206"/>
-      <c r="R4" s="208"/>
+      <c r="P4" s="232"/>
+      <c r="Q4" s="234"/>
+      <c r="R4" s="236"/>
       <c r="AE4" s="146"/>
     </row>
     <row r="5" spans="1:31" ht="44.25" customHeight="1">
-      <c r="A5" s="225"/>
-      <c r="B5" s="216"/>
-      <c r="C5" s="217"/>
-      <c r="D5" s="208"/>
+      <c r="A5" s="252"/>
+      <c r="B5" s="246"/>
+      <c r="C5" s="247"/>
+      <c r="D5" s="236"/>
       <c r="E5" s="134" t="s">
         <v>8</v>
       </c>
@@ -18752,7 +19696,7 @@
       <c r="O5" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="218"/>
+      <c r="P5" s="232"/>
       <c r="Q5" s="148"/>
       <c r="R5" s="148"/>
     </row>
@@ -18760,10 +19704,10 @@
       <c r="A6" s="132" t="s">
         <v>311</v>
       </c>
-      <c r="B6" s="221" t="s">
+      <c r="B6" s="249" t="s">
         <v>412</v>
       </c>
-      <c r="C6" s="221"/>
+      <c r="C6" s="249"/>
       <c r="D6" s="132">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -19153,10 +20097,10 @@
       <c r="A13" s="132" t="s">
         <v>317</v>
       </c>
-      <c r="B13" s="222" t="s">
+      <c r="B13" s="250" t="s">
         <v>413</v>
       </c>
-      <c r="C13" s="222"/>
+      <c r="C13" s="250"/>
       <c r="D13" s="134">
         <f>+D14+D25</f>
         <v>3300</v>
@@ -19216,10 +20160,10 @@
       <c r="A14" s="132" t="s">
         <v>415</v>
       </c>
-      <c r="B14" s="221" t="s">
+      <c r="B14" s="249" t="s">
         <v>414</v>
       </c>
-      <c r="C14" s="223"/>
+      <c r="C14" s="251"/>
       <c r="D14" s="149">
         <f>+SUM(D15:D24)</f>
         <v>860</v>
@@ -19825,10 +20769,10 @@
       <c r="A25" s="132" t="s">
         <v>416</v>
       </c>
-      <c r="B25" s="221" t="s">
+      <c r="B25" s="249" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="221"/>
+      <c r="C25" s="249"/>
       <c r="D25" s="149">
         <f>+SUM(D26:D46)</f>
         <v>2440</v>
@@ -20958,10 +21902,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" ht="20.25" customHeight="1">
-      <c r="A47" s="210" t="s">
+      <c r="A47" s="240" t="s">
         <v>418</v>
       </c>
-      <c r="B47" s="211"/>
+      <c r="B47" s="241"/>
       <c r="C47" s="148"/>
       <c r="D47" s="128">
         <f>SUM(D6,D13)</f>
@@ -20984,10 +21928,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="B3:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -20996,11 +21936,15 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A2:P2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="D3:G3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:P2"/>
     <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="76" orientation="portrait" r:id="rId1"/>
@@ -21014,7 +21958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -21025,207 +21969,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="234">
+      <c r="A1" s="189">
         <v>1</v>
       </c>
-      <c r="B1" s="232" t="s">
+      <c r="B1" s="187" t="s">
         <v>435</v>
       </c>
-      <c r="C1" s="232">
+      <c r="C1" s="187">
         <f>H1</f>
         <v>24</v>
       </c>
-      <c r="D1" s="232">
+      <c r="D1" s="187">
         <v>6</v>
       </c>
-      <c r="E1" s="232">
+      <c r="E1" s="187">
         <v>16</v>
       </c>
-      <c r="F1" s="232">
+      <c r="F1" s="187">
         <v>2</v>
       </c>
-      <c r="H1" s="236">
+      <c r="H1" s="191">
         <f>SUM(D1:F1)</f>
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18">
-      <c r="A2" s="234">
+      <c r="A2" s="189">
         <v>2</v>
       </c>
-      <c r="B2" s="232" t="s">
+      <c r="B2" s="187" t="s">
         <v>436</v>
       </c>
-      <c r="C2" s="232">
+      <c r="C2" s="187">
         <f t="shared" ref="C2:C4" si="0">H2</f>
         <v>24</v>
       </c>
-      <c r="D2" s="232">
+      <c r="D2" s="187">
         <v>6</v>
       </c>
-      <c r="E2" s="232">
+      <c r="E2" s="187">
         <v>17</v>
       </c>
-      <c r="F2" s="232">
+      <c r="F2" s="187">
         <v>1</v>
       </c>
-      <c r="H2" s="236">
+      <c r="H2" s="191">
         <f t="shared" ref="H2:H4" si="1">SUM(D2:F2)</f>
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18">
-      <c r="A3" s="234">
+      <c r="A3" s="189">
         <v>3</v>
       </c>
-      <c r="B3" s="232" t="s">
+      <c r="B3" s="187" t="s">
         <v>437</v>
       </c>
-      <c r="C3" s="232">
+      <c r="C3" s="187">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="D3" s="232">
+      <c r="D3" s="187">
         <v>32</v>
       </c>
-      <c r="E3" s="232">
+      <c r="E3" s="187">
         <v>48</v>
       </c>
-      <c r="F3" s="232">
+      <c r="F3" s="187">
         <v>4</v>
       </c>
-      <c r="H3" s="236">
+      <c r="H3" s="191">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="K3" s="235">
+      <c r="K3" s="190">
         <f>SUM(L3:N3)</f>
         <v>36</v>
       </c>
-      <c r="L3" s="232">
+      <c r="L3" s="187">
         <v>6</v>
       </c>
-      <c r="M3" s="232">
+      <c r="M3" s="187">
         <v>28</v>
       </c>
-      <c r="N3" s="232">
+      <c r="N3" s="187">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18">
-      <c r="A4" s="234">
+      <c r="A4" s="189">
         <v>4</v>
       </c>
-      <c r="B4" s="232" t="s">
+      <c r="B4" s="187" t="s">
         <v>438</v>
       </c>
-      <c r="C4" s="232">
+      <c r="C4" s="187">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D4" s="232">
+      <c r="D4" s="187">
         <v>6</v>
       </c>
-      <c r="E4" s="232">
+      <c r="E4" s="187">
         <v>10</v>
       </c>
-      <c r="F4" s="232">
+      <c r="F4" s="187">
         <v>2</v>
       </c>
-      <c r="H4" s="236">
+      <c r="H4" s="191">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18">
-      <c r="A5" s="234">
+      <c r="A5" s="189">
         <v>4</v>
       </c>
-      <c r="B5" s="232" t="s">
+      <c r="B5" s="187" t="s">
         <v>439</v>
       </c>
-      <c r="C5" s="232">
+      <c r="C5" s="187">
         <f t="shared" ref="C5" si="2">H5</f>
         <v>30</v>
       </c>
-      <c r="D5" s="232">
-        <v>0</v>
-      </c>
-      <c r="E5" s="232">
+      <c r="D5" s="187">
+        <v>0</v>
+      </c>
+      <c r="E5" s="187">
         <v>30</v>
       </c>
-      <c r="F5" s="232">
-        <v>0</v>
-      </c>
-      <c r="H5" s="236">
+      <c r="F5" s="187">
+        <v>0</v>
+      </c>
+      <c r="H5" s="191">
         <f t="shared" ref="H5" si="3">SUM(D5:F5)</f>
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18">
-      <c r="C6" s="233">
+      <c r="C6" s="188">
         <f>SUM(C1:C5)</f>
         <v>180</v>
       </c>
-      <c r="D6" s="233">
+      <c r="D6" s="188">
         <f t="shared" ref="D6:F6" si="4">SUM(D1:D5)</f>
         <v>50</v>
       </c>
-      <c r="E6" s="233">
+      <c r="E6" s="188">
         <f t="shared" si="4"/>
         <v>121</v>
       </c>
-      <c r="F6" s="233">
+      <c r="F6" s="188">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="H6" s="235">
+      <c r="H6" s="190">
         <f>SUM(D6:F6)</f>
         <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18">
-      <c r="C7" s="233"/>
-      <c r="D7" s="233"/>
-      <c r="E7" s="233"/>
-      <c r="F7" s="233"/>
-      <c r="H7" s="235"/>
-    </row>
-    <row r="8" spans="1:14" s="238" customFormat="1">
-      <c r="C8" s="238" t="s">
+      <c r="C7" s="188"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="H7" s="190"/>
+    </row>
+    <row r="8" spans="1:14" s="193" customFormat="1">
+      <c r="C8" s="193" t="s">
         <v>451</v>
       </c>
-      <c r="G8" s="239"/>
-    </row>
-    <row r="9" spans="1:14" s="238" customFormat="1" ht="28.8">
-      <c r="B9" s="238">
+      <c r="G8" s="194"/>
+    </row>
+    <row r="9" spans="1:14" s="193" customFormat="1" ht="28.8">
+      <c r="B9" s="193">
         <f>SUM(C10,C16)</f>
         <v>24</v>
       </c>
-      <c r="C9" s="240" t="s">
+      <c r="C9" s="195" t="s">
         <v>453</v>
       </c>
-      <c r="D9" s="240" t="s">
+      <c r="D9" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="240" t="s">
+      <c r="E9" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="240" t="s">
+      <c r="F9" s="195" t="s">
         <v>454</v>
       </c>
-      <c r="G9" s="241" t="s">
+      <c r="G9" s="196" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="242">
+      <c r="A10" s="197">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>440</v>
       </c>
-      <c r="C10" s="238">
+      <c r="C10" s="193">
         <f>SUM(D10:F10)</f>
         <v>8</v>
       </c>
@@ -21243,13 +22187,13 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="242">
+      <c r="A11" s="197">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>441</v>
       </c>
-      <c r="C11" s="238">
+      <c r="C11" s="193">
         <f>SUM(D11:F11)</f>
         <v>0.5</v>
       </c>
@@ -21258,13 +22202,13 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="242">
+      <c r="A12" s="197">
         <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>443</v>
       </c>
-      <c r="C12" s="238">
+      <c r="C12" s="193">
         <f t="shared" ref="C12:C15" si="6">SUM(D12:F12)</f>
         <v>2</v>
       </c>
@@ -21276,13 +22220,13 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="242">
+      <c r="A13" s="197">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>444</v>
       </c>
-      <c r="C13" s="238">
+      <c r="C13" s="193">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
@@ -21294,13 +22238,13 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="242">
+      <c r="A14" s="197">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>445</v>
       </c>
-      <c r="C14" s="238">
+      <c r="C14" s="193">
         <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
@@ -21309,13 +22253,13 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="242">
+      <c r="A15" s="197">
         <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>446</v>
       </c>
-      <c r="C15" s="238">
+      <c r="C15" s="193">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
@@ -21330,13 +22274,13 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="242">
+      <c r="A16" s="197">
         <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>442</v>
       </c>
-      <c r="C16" s="238">
+      <c r="C16" s="193">
         <f>SUM(C17:C21)</f>
         <v>16</v>
       </c>
@@ -21354,13 +22298,13 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="242">
+      <c r="A17" s="197">
         <v>8</v>
       </c>
-      <c r="B17" s="237" t="s">
+      <c r="B17" s="192" t="s">
         <v>447</v>
       </c>
-      <c r="C17" s="238">
+      <c r="C17" s="193">
         <f>SUM(D17:F17)</f>
         <v>1</v>
       </c>
@@ -21369,13 +22313,13 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="242">
+      <c r="A18" s="197">
         <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>448</v>
       </c>
-      <c r="C18" s="238">
+      <c r="C18" s="193">
         <f t="shared" ref="C18:C21" si="8">SUM(D18:F18)</f>
         <v>1</v>
       </c>
@@ -21384,13 +22328,13 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="242">
+      <c r="A19" s="197">
         <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>449</v>
       </c>
-      <c r="C19" s="238">
+      <c r="C19" s="193">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -21399,13 +22343,13 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="242">
+      <c r="A20" s="197">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>450</v>
       </c>
-      <c r="C20" s="238">
+      <c r="C20" s="193">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
@@ -21414,13 +22358,13 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="242">
+      <c r="A21" s="197">
         <v>12</v>
       </c>
       <c r="B21" t="s">
         <v>455</v>
       </c>
-      <c r="C21" s="238">
+      <c r="C21" s="193">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
@@ -21432,107 +22376,107 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="238"/>
-      <c r="B24" s="238"/>
-      <c r="C24" s="238" t="s">
+      <c r="A24" s="193"/>
+      <c r="B24" s="193"/>
+      <c r="C24" s="193" t="s">
         <v>451</v>
       </c>
-      <c r="D24" s="238"/>
-      <c r="E24" s="238"/>
-      <c r="F24" s="238"/>
-      <c r="G24" s="239"/>
+      <c r="D24" s="193"/>
+      <c r="E24" s="193"/>
+      <c r="F24" s="193"/>
+      <c r="G24" s="194"/>
     </row>
     <row r="25" spans="1:7" ht="28.8">
-      <c r="A25" s="238"/>
-      <c r="B25" s="238"/>
-      <c r="C25" s="240" t="s">
+      <c r="A25" s="193"/>
+      <c r="B25" s="193"/>
+      <c r="C25" s="195" t="s">
         <v>453</v>
       </c>
-      <c r="D25" s="240" t="s">
+      <c r="D25" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="240" t="s">
+      <c r="E25" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="240" t="s">
+      <c r="F25" s="195" t="s">
         <v>454</v>
       </c>
-      <c r="G25" s="241" t="s">
+      <c r="G25" s="196" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="242">
+      <c r="A26" s="197">
         <v>1</v>
       </c>
-      <c r="C26" s="238"/>
+      <c r="C26" s="193"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="242">
+      <c r="A27" s="197">
         <v>2</v>
       </c>
-      <c r="C27" s="238"/>
+      <c r="C27" s="193"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="242">
+      <c r="A28" s="197">
         <v>3</v>
       </c>
-      <c r="C28" s="238"/>
+      <c r="C28" s="193"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="242">
+      <c r="A29" s="197">
         <v>4</v>
       </c>
-      <c r="C29" s="238"/>
+      <c r="C29" s="193"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="242">
+      <c r="A30" s="197">
         <v>5</v>
       </c>
-      <c r="C30" s="238"/>
+      <c r="C30" s="193"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="242">
+      <c r="A31" s="197">
         <v>6</v>
       </c>
-      <c r="C31" s="238"/>
+      <c r="C31" s="193"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="242">
+      <c r="A32" s="197">
         <v>7</v>
       </c>
-      <c r="C32" s="238"/>
+      <c r="C32" s="193"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="242">
+      <c r="A33" s="197">
         <v>8</v>
       </c>
-      <c r="B33" s="237"/>
-      <c r="C33" s="238"/>
+      <c r="B33" s="192"/>
+      <c r="C33" s="193"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="242">
+      <c r="A34" s="197">
         <v>9</v>
       </c>
-      <c r="C34" s="238"/>
+      <c r="C34" s="193"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="242">
+      <c r="A35" s="197">
         <v>10</v>
       </c>
-      <c r="C35" s="238"/>
+      <c r="C35" s="193"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="242">
+      <c r="A36" s="197">
         <v>11</v>
       </c>
-      <c r="C36" s="238"/>
+      <c r="C36" s="193"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="242">
+      <c r="A37" s="197">
         <v>12</v>
       </c>
-      <c r="C37" s="238"/>
+      <c r="C37" s="193"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21542,440 +22486,204 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="48.109375" customWidth="1"/>
+    <col min="1" max="1" width="66.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A1" s="227" t="s">
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="193">
+        <v>30</v>
+      </c>
+      <c r="I1" s="193">
+        <v>6</v>
+      </c>
+      <c r="J1" s="193">
+        <v>22</v>
+      </c>
+      <c r="K1" s="193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="193" customFormat="1">
+      <c r="A2" s="193" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" s="193">
+        <f>SUM(B3:B4)</f>
+        <v>7</v>
+      </c>
+      <c r="C2" s="193">
+        <f>SUM(C3:C4)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="193">
+        <f>SUM(D3:D4)</f>
+        <v>4</v>
+      </c>
+      <c r="E2" s="193">
+        <f>SUM(E3:E4)</f>
         <v>1</v>
       </c>
-      <c r="B1" s="227" t="s">
-        <v>307</v>
-      </c>
-      <c r="C1" s="229" t="s">
-        <v>308</v>
-      </c>
-      <c r="D1" s="230"/>
-      <c r="E1" s="230"/>
-      <c r="F1" s="231"/>
-    </row>
-    <row r="2" spans="1:6" ht="51" thickBot="1">
-      <c r="A2" s="228"/>
-      <c r="B2" s="228"/>
-      <c r="C2" s="107" t="s">
-        <v>309</v>
-      </c>
-      <c r="D2" s="107" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B8" si="0">SUM(C3:E3)</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8">
+      <c r="A4" s="198" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="193" customFormat="1">
+      <c r="A5" s="193" t="s">
+        <v>458</v>
+      </c>
+      <c r="B5" s="193">
+        <f>SUM(B6:B9)</f>
+        <v>23</v>
+      </c>
+      <c r="C5" s="193">
+        <f>SUM(C6:C9)</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="193">
+        <f>SUM(D6:D9)</f>
+        <v>18</v>
+      </c>
+      <c r="E5" s="193">
+        <f>SUM(E6:E9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>459</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>8</v>
       </c>
-      <c r="E2" s="107" t="s">
-        <v>310</v>
-      </c>
-      <c r="F2" s="107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A3" s="108" t="s">
-        <v>311</v>
-      </c>
-      <c r="B3" s="109" t="s">
-        <v>312</v>
-      </c>
-      <c r="C3" s="107">
-        <f>SUM(D3:F3)</f>
-        <v>5</v>
-      </c>
-      <c r="D3" s="107">
-        <f>SUM(D4:D7)</f>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>460</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E3" s="107">
-        <f t="shared" ref="E3" si="0">SUM(E4:E7)</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="107"/>
-    </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A4" s="111">
-        <v>1</v>
-      </c>
-      <c r="B4" s="112" t="s">
-        <v>313</v>
-      </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="114">
-        <v>1</v>
-      </c>
-      <c r="E4" s="113"/>
-      <c r="F4" s="110"/>
-    </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A5" s="111">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>461</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>462</v>
+      </c>
+      <c r="B10" s="193">
+        <f>SUM(B2:B9)/2</f>
+        <v>30</v>
+      </c>
+      <c r="C10" s="193">
+        <f>SUM(C5,C2)</f>
+        <v>6</v>
+      </c>
+      <c r="D10" s="193">
+        <f>SUM(D5,D2)</f>
+        <v>22</v>
+      </c>
+      <c r="E10" s="193">
+        <f>SUM(E5,E2)</f>
         <v>2</v>
       </c>
-      <c r="B5" s="112" t="s">
-        <v>314</v>
-      </c>
-      <c r="C5" s="113"/>
-      <c r="D5" s="114">
-        <v>1</v>
-      </c>
-      <c r="E5" s="113"/>
-      <c r="F5" s="110"/>
-    </row>
-    <row r="6" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A6" s="111">
-        <v>3</v>
-      </c>
-      <c r="B6" s="112" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="114">
-        <v>1</v>
-      </c>
-      <c r="E6" s="113"/>
-      <c r="F6" s="110"/>
-    </row>
-    <row r="7" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A7" s="111">
-        <v>4</v>
-      </c>
-      <c r="B7" s="112" t="s">
-        <v>316</v>
-      </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="114">
-        <v>1</v>
-      </c>
-      <c r="E7" s="114">
-        <v>1</v>
-      </c>
-      <c r="F7" s="110"/>
-    </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A8" s="108" t="s">
-        <v>317</v>
-      </c>
-      <c r="B8" s="109" t="s">
-        <v>318</v>
-      </c>
-      <c r="C8" s="107">
-        <f>SUM(D8:F8)</f>
-        <v>16</v>
-      </c>
-      <c r="D8" s="107">
-        <f>SUM(D9:D11)</f>
-        <v>9</v>
-      </c>
-      <c r="E8" s="107">
-        <f t="shared" ref="E8" si="1">SUM(E9:E11)</f>
-        <v>6</v>
-      </c>
-      <c r="F8" s="107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34.200000000000003" thickBot="1">
-      <c r="A9" s="111">
-        <v>1</v>
-      </c>
-      <c r="B9" s="112" t="s">
-        <v>319</v>
-      </c>
-      <c r="C9" s="113"/>
-      <c r="D9" s="114">
-        <v>1</v>
-      </c>
-      <c r="E9" s="114">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="110"/>
-    </row>
-    <row r="10" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A10" s="111">
-        <v>2</v>
-      </c>
-      <c r="B10" s="112" t="s">
-        <v>320</v>
-      </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="114">
-        <v>1</v>
-      </c>
-      <c r="E10" s="114">
-        <v>1</v>
-      </c>
-      <c r="F10" s="110"/>
-    </row>
-    <row r="11" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A11" s="111">
-        <v>3</v>
-      </c>
-      <c r="B11" s="112" t="s">
-        <v>321</v>
-      </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="114">
-        <v>7</v>
-      </c>
-      <c r="E11" s="114">
-        <v>4.5</v>
-      </c>
-      <c r="F11" s="110"/>
-    </row>
-    <row r="12" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A12" s="108" t="s">
-        <v>322</v>
-      </c>
-      <c r="B12" s="109" t="s">
-        <v>323</v>
-      </c>
-      <c r="C12" s="107">
-        <f>SUM(D12:F12)</f>
-        <v>17</v>
-      </c>
-      <c r="D12" s="107">
-        <f>SUM(D13:D16)</f>
-        <v>11</v>
-      </c>
-      <c r="E12" s="107">
-        <f t="shared" ref="E12" si="2">SUM(E13:E16)</f>
-        <v>5</v>
-      </c>
-      <c r="F12" s="107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A13" s="111">
-        <v>1</v>
-      </c>
-      <c r="B13" s="112" t="s">
-        <v>324</v>
-      </c>
-      <c r="C13" s="113"/>
-      <c r="D13" s="114">
-        <v>1</v>
-      </c>
-      <c r="E13" s="114">
-        <v>1</v>
-      </c>
-      <c r="F13" s="110"/>
-    </row>
-    <row r="14" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A14" s="111">
-        <v>2</v>
-      </c>
-      <c r="B14" s="112" t="s">
-        <v>325</v>
-      </c>
-      <c r="C14" s="113"/>
-      <c r="D14" s="114">
-        <v>3</v>
-      </c>
-      <c r="E14" s="114">
-        <v>1</v>
-      </c>
-      <c r="F14" s="110"/>
-    </row>
-    <row r="15" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A15" s="111">
-        <v>3</v>
-      </c>
-      <c r="B15" s="112" t="s">
-        <v>326</v>
-      </c>
-      <c r="C15" s="113"/>
-      <c r="D15" s="114">
-        <v>3</v>
-      </c>
-      <c r="E15" s="114">
-        <v>1</v>
-      </c>
-      <c r="F15" s="110"/>
-    </row>
-    <row r="16" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A16" s="111">
-        <v>4</v>
-      </c>
-      <c r="B16" s="112" t="s">
-        <v>327</v>
-      </c>
-      <c r="C16" s="113"/>
-      <c r="D16" s="114">
-        <v>4</v>
-      </c>
-      <c r="E16" s="114">
-        <v>2</v>
-      </c>
-      <c r="F16" s="110"/>
-    </row>
-    <row r="17" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A17" s="108" t="s">
-        <v>328</v>
-      </c>
-      <c r="B17" s="109" t="s">
-        <v>329</v>
-      </c>
-      <c r="C17" s="107">
-        <f>SUM(D17:F17)</f>
-        <v>17</v>
-      </c>
-      <c r="D17" s="107">
-        <f>SUM(D18:D20)</f>
-        <v>10</v>
-      </c>
-      <c r="E17" s="107">
-        <f>SUM(E18:E20)</f>
-        <v>6</v>
-      </c>
-      <c r="F17" s="115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A18" s="111">
-        <v>1</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>330</v>
-      </c>
-      <c r="C18" s="113"/>
-      <c r="D18" s="114">
-        <v>4</v>
-      </c>
-      <c r="E18" s="114">
-        <v>3</v>
-      </c>
-      <c r="F18" s="110"/>
-    </row>
-    <row r="19" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A19" s="111">
-        <v>3</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>331</v>
-      </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="114">
-        <v>3</v>
-      </c>
-      <c r="E19" s="114">
-        <v>1</v>
-      </c>
-      <c r="F19" s="110"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A20" s="111">
-        <v>4</v>
-      </c>
-      <c r="B20" s="112" t="s">
-        <v>332</v>
-      </c>
-      <c r="C20" s="113"/>
-      <c r="D20" s="114">
-        <v>3</v>
-      </c>
-      <c r="E20" s="114">
-        <v>2</v>
-      </c>
-      <c r="F20" s="110"/>
-    </row>
-    <row r="21" spans="1:6" ht="34.200000000000003" thickBot="1">
-      <c r="A21" s="108" t="s">
-        <v>333</v>
-      </c>
-      <c r="B21" s="109" t="s">
-        <v>334</v>
-      </c>
-      <c r="C21" s="107">
-        <f>SUM(D21:F21)</f>
-        <v>5</v>
-      </c>
-      <c r="D21" s="107">
-        <f>SUM(D22:D23)</f>
-        <v>2</v>
-      </c>
-      <c r="E21" s="107">
-        <f>SUM(E22:E23)</f>
-        <v>2</v>
-      </c>
-      <c r="F21" s="115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A22" s="111">
-        <v>1</v>
-      </c>
-      <c r="B22" s="112" t="s">
-        <v>335</v>
-      </c>
-      <c r="C22" s="113"/>
-      <c r="D22" s="114">
-        <v>1</v>
-      </c>
-      <c r="E22" s="114">
-        <v>1</v>
-      </c>
-      <c r="F22" s="110"/>
-    </row>
-    <row r="23" spans="1:6" ht="34.200000000000003" thickBot="1">
-      <c r="A23" s="111">
-        <v>2</v>
-      </c>
-      <c r="B23" s="112" t="s">
-        <v>336</v>
-      </c>
-      <c r="C23" s="113"/>
-      <c r="D23" s="114">
-        <v>1</v>
-      </c>
-      <c r="E23" s="114">
-        <v>1</v>
-      </c>
-      <c r="F23" s="110"/>
-    </row>
-    <row r="24" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A24" s="229" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="231"/>
-      <c r="C24" s="107">
-        <f>SUM(C3,C8,C12,C17,C21)</f>
-        <v>60</v>
-      </c>
-      <c r="D24" s="107">
-        <f>SUM(D3,D8,D12,D17,D21)</f>
-        <v>36</v>
-      </c>
-      <c r="E24" s="107">
-        <f>SUM(E3,E8,E12,E17,E21)</f>
-        <v>20</v>
-      </c>
-      <c r="F24" s="107">
-        <f>SUM(F3,F8,F12,F17,F21)</f>
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A24:B24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update chương trình chi tiết, phân tích nghề
</commit_message>
<xml_diff>
--- a/So sanh CTTĐ.xlsx
+++ b/So sanh CTTĐ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21864" windowHeight="11040" firstSheet="8" activeTab="12"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21864" windowHeight="11040" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="CGKL" sheetId="1" state="hidden" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="đo lường điện tử" sheetId="8" r:id="rId12"/>
     <sheet name="DienTuNangcao" sheetId="14" r:id="rId13"/>
     <sheet name="Điện tử nâng cao" sheetId="10" r:id="rId14"/>
+    <sheet name="KTTTS" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc453594266" localSheetId="12">DienTuNangcao!$A$4</definedName>
@@ -185,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="594">
   <si>
     <t>SO SÁNH CHƯƠNG TRÌNH ĐÀO TẠO NGHỀ CẮT GỌT KIM LOẠI</t>
   </si>
@@ -1794,6 +1796,213 @@
   </si>
   <si>
     <t>5. Một số mạch dùng IC và cảm biến</t>
+  </si>
+  <si>
+    <t>Bài 1:  Tổng quan về kỹ thuật truyền thông số</t>
+  </si>
+  <si>
+    <t>Khái quát lịch sử phát triển của thông truyền thông số</t>
+  </si>
+  <si>
+    <t>Tại sao cần phải truyền thông và truyền thông ra đời như thế nào</t>
+  </si>
+  <si>
+    <t>Các thành phần cơ bản hệ thống truyền thông số</t>
+  </si>
+  <si>
+    <t>Bài 2: Một số khái niệm cơ bản</t>
+  </si>
+  <si>
+    <t>Nguồn tin, kênh tin, nhận tin, nhiễu</t>
+  </si>
+  <si>
+    <t>Sơ đồ khối một hệ thống thông tin số</t>
+  </si>
+  <si>
+    <t>Các phương thức liên lạc : Đơn công, bán song công, song công</t>
+  </si>
+  <si>
+    <t>Bài 3 :Hướng dẫn sử dụng phần mềm mô phỏng và xử lý tín hiệu Matlab Simulink</t>
+  </si>
+  <si>
+    <t>Cài đặt phần mềm mô phỏng Matlab Simulink</t>
+  </si>
+  <si>
+    <t>Làm việc trực tiếp với môi trường command window</t>
+  </si>
+  <si>
+    <t>Biểu diễn tín hiệu theo phương pháp liệt kê</t>
+  </si>
+  <si>
+    <t>Biểu diễn một véc tơ thời gian, biểu diễn tín hiệu theo phương pháp sử dụng bước nhảy default và bước nhảy xác định</t>
+  </si>
+  <si>
+    <t>Bài tập áp dụng biểu diễn tín hiệu</t>
+  </si>
+  <si>
+    <t>Bài 4 : Các phép toán về véc tơ trong xử lý tín hiệu</t>
+  </si>
+  <si>
+    <t>Biểu diễn một véc tơ thời gian theo phương pháp tuyến tính linspace</t>
+  </si>
+  <si>
+    <t>Một số phép toán với véc tơ ứng dụng trong xử lý tín hiệu</t>
+  </si>
+  <si>
+    <t>Sử dụng Script tạo function</t>
+  </si>
+  <si>
+    <t>Bài tập áp dụng xử lý tín hiệu</t>
+  </si>
+  <si>
+    <t>Kiểm tra 1 tiết</t>
+  </si>
+  <si>
+    <t>Bài 5 : Các phép toán về ma trận trong xử lý tín hiệu</t>
+  </si>
+  <si>
+    <t>Một số phép toán với ma trận ứng dụng trong xử lý tín hiệu</t>
+  </si>
+  <si>
+    <t>Bài 6 : Xử lý một số tín hiệu và biểu diễn dãy cơ bản</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lập trình vẽ đồ thị hàm xung đơn vị Impulse Signal </t>
+  </si>
+  <si>
+    <t>Vẽ đồ thị hàm bước nhảy step Signal</t>
+  </si>
+  <si>
+    <t>Lập trình vẽ đồ thị hàm dãy chữ nhật rectangle Signal rectN(t)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bài 7 : Biểu diễn đặc tính tín hiệu </t>
+  </si>
+  <si>
+    <t>Biểu diễn hàm trễ theo thời gian</t>
+  </si>
+  <si>
+    <t>Biểu diễn nhiều tín hiệu trên cùng một mặt phẳng tọa độ</t>
+  </si>
+  <si>
+    <t>Biểu diễn nhiều tín hiệu trên nhiều trục tọa độ khác nhau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bài 8 : Biểu diễn đặc tính tín hiệu </t>
+  </si>
+  <si>
+    <t>Phương pháp biểu diễn tín hiệu bằng cách thiết lập đặc tính linewidth</t>
+  </si>
+  <si>
+    <t>Phương pháp biểu diễn tín hiệu bằng cách thiết lập đặc tính colour</t>
+  </si>
+  <si>
+    <t>Bài tập áp dụng</t>
+  </si>
+  <si>
+    <t>Bài 9 : Hệ thống tuyến tính bất biến</t>
+  </si>
+  <si>
+    <t>Định nghĩa và cách xác định</t>
+  </si>
+  <si>
+    <t>Tính tích chập bằng phương pháp đồ thị</t>
+  </si>
+  <si>
+    <t>Tính tích chập bằng phương pháp dùng bảng</t>
+  </si>
+  <si>
+    <t>Tính tích chập bằng phương pháp dùng lệnh trong Matlab</t>
+  </si>
+  <si>
+    <t>Kiểm tra mô phỏng xử lý tín hiệu</t>
+  </si>
+  <si>
+    <t>Bài 10: Các phép biểu diễn và biến đổi hệ thống tuyến tính</t>
+  </si>
+  <si>
+    <t>Biểu diễn hệ thống tuyến tính bất biến bằng phương trình sai phân và bằng sơ đồ</t>
+  </si>
+  <si>
+    <t>Bài tập xác định hệ thống tuyến tính và thực hành tính tích chập</t>
+  </si>
+  <si>
+    <t>Kiểm tra tính tích chập bằng phương pháp đồ thị</t>
+  </si>
+  <si>
+    <t>Bài 11: Một số đặc tính của xung</t>
+  </si>
+  <si>
+    <t>Trình bày, phân tích các chức năng cơ bản của máy hiện sóng để đo các đặc tính của xung</t>
+  </si>
+  <si>
+    <t>Xác định biên độ xung Um</t>
+  </si>
+  <si>
+    <t>Độ rộng xung Tx là gì và cách đo</t>
+  </si>
+  <si>
+    <t>Xác định chu kỳ xung, tần số xung</t>
+  </si>
+  <si>
+    <t>Ý nghĩa của độ rộng sườn trước rising time và cách xác định</t>
+  </si>
+  <si>
+    <t>Xác định độ rộng sườn sau falling time</t>
+  </si>
+  <si>
+    <t>Bài 12: Điều chế biên độ xung Pulse Amplitude Modulation</t>
+  </si>
+  <si>
+    <t>Cấu tạo, nguyên lý hoạt động của mô đun điều chế tín hiệu xung theo biên độ PAM: cách cấp nguồn, cách lấy tín hiệu ngõ ra.</t>
+  </si>
+  <si>
+    <t>Nguyên lý hoạt động và cách kết nối của mô đun: Power Supply 2920A, Signal Soure 2920B.</t>
+  </si>
+  <si>
+    <t>Phương pháp tạo xung PAM và định lý lấy mẫu Nyquist–Shannon</t>
+  </si>
+  <si>
+    <t>Đo và phân tích ảnh hưởng của tần số trích mẫu Fs lên tín hiệu PAM</t>
+  </si>
+  <si>
+    <t>Đo và phân tích ảnh hưởng của Fcut off lên Low pass filter</t>
+  </si>
+  <si>
+    <t>Bài 13: Điều chế độ rộng xung Pulse Width Modulation</t>
+  </si>
+  <si>
+    <t>Một số phương pháp tạo ra PWM</t>
+  </si>
+  <si>
+    <t>Đo và xác định một số đặc tính của PWM trên kit truyền thông 2920</t>
+  </si>
+  <si>
+    <t>Lập trình mô phỏng, vẽ đồ thị điều chế PAM</t>
+  </si>
+  <si>
+    <t>Viết chương trình điều khiển PAM bằng Matlab Simulink</t>
+  </si>
+  <si>
+    <t>* Kiểm tra kết thúc môn</t>
+  </si>
+  <si>
+    <t>Bài 14: Bài tập lớn</t>
+  </si>
+  <si>
+    <t>Bài 1: Giới thiệu hệ thống điều khiển điện khí nén</t>
+  </si>
+  <si>
+    <t>Bài 2: Các phần tử trong hệ thống điện khí nén</t>
+  </si>
+  <si>
+    <t>Bài 3: Thiết kế, lắp đặt và vận hành hệ thống điện khí nén</t>
+  </si>
+  <si>
+    <t>Bài 4: Tìm và sửa lỗi trong hệ thống điều khiển điện – khí nén</t>
+  </si>
+  <si>
+    <t>Kiểm tra kết thúc mô đun</t>
   </si>
 </sst>
 </file>
@@ -2431,7 +2640,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2975,6 +3184,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3451,59 +3664,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
+      <c r="A2" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="221" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221" t="s">
+      <c r="C3" s="223"/>
+      <c r="D3" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="222" t="s">
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="222" t="s">
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="224" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="221"/>
+      <c r="A4" s="223"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -3546,7 +3759,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="222"/>
+      <c r="P4" s="224"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -3579,10 +3792,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="213" t="s">
+      <c r="B6" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -3917,10 +4130,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="215" t="s">
+      <c r="B13" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="216"/>
+      <c r="C13" s="218"/>
       <c r="D13" s="18">
         <f>+D14+D27</f>
         <v>2355</v>
@@ -3943,10 +4156,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8"/>
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="218"/>
+      <c r="C14" s="220"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D26)</f>
         <v>570</v>
@@ -4584,10 +4797,10 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="8"/>
-      <c r="B27" s="219" t="s">
+      <c r="B27" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="219"/>
+      <c r="C27" s="221"/>
       <c r="D27" s="22">
         <f>+SUM(D28:D50)</f>
         <v>1785</v>
@@ -4848,23 +5061,23 @@
       <c r="K32" s="14">
         <v>3</v>
       </c>
-      <c r="L32" s="226">
+      <c r="L32" s="228">
         <f>+H32+H33+H34-D32-D33-D34-D35-D39-D41-D42-D43-D52-D53</f>
         <v>-365</v>
       </c>
-      <c r="M32" s="226">
+      <c r="M32" s="228">
         <f t="shared" ref="M32:O32" si="7">+I32+I33+I34-E32-E33-E34-E35-E39-E41-E42-E43-E52-E53</f>
         <v>-77</v>
       </c>
-      <c r="N32" s="226">
+      <c r="N32" s="228">
         <f t="shared" si="7"/>
         <v>-276</v>
       </c>
-      <c r="O32" s="226">
+      <c r="O32" s="228">
         <f t="shared" si="7"/>
         <v>-12</v>
       </c>
-      <c r="P32" s="226" t="s">
+      <c r="P32" s="228" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4902,11 +5115,11 @@
       <c r="K33" s="14">
         <v>3</v>
       </c>
-      <c r="L33" s="227"/>
-      <c r="M33" s="227"/>
-      <c r="N33" s="227"/>
-      <c r="O33" s="227"/>
-      <c r="P33" s="227"/>
+      <c r="L33" s="229"/>
+      <c r="M33" s="229"/>
+      <c r="N33" s="229"/>
+      <c r="O33" s="229"/>
+      <c r="P33" s="229"/>
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="33">
@@ -4942,11 +5155,11 @@
       <c r="K34" s="14">
         <v>4</v>
       </c>
-      <c r="L34" s="228"/>
-      <c r="M34" s="228"/>
-      <c r="N34" s="228"/>
-      <c r="O34" s="228"/>
-      <c r="P34" s="228"/>
+      <c r="L34" s="230"/>
+      <c r="M34" s="230"/>
+      <c r="N34" s="230"/>
+      <c r="O34" s="230"/>
+      <c r="P34" s="230"/>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="33">
@@ -4982,23 +5195,23 @@
       <c r="K35" s="14">
         <v>3</v>
       </c>
-      <c r="L35" s="226">
+      <c r="L35" s="228">
         <f>+H35+H36-D36-D37-D38-D44-D45-D46-D54-D55-D56-D57-D58</f>
         <v>-500</v>
       </c>
-      <c r="M35" s="226">
+      <c r="M35" s="228">
         <f t="shared" ref="M35:O35" si="8">+I35+I36-E36-E37-E38-E44-E45-E46-E54-E55-E56-E57-E58</f>
         <v>-65</v>
       </c>
-      <c r="N35" s="226">
+      <c r="N35" s="228">
         <f t="shared" si="8"/>
         <v>-422</v>
       </c>
-      <c r="O35" s="226">
+      <c r="O35" s="228">
         <f t="shared" si="8"/>
         <v>-13</v>
       </c>
-      <c r="P35" s="226" t="s">
+      <c r="P35" s="228" t="s">
         <v>100</v>
       </c>
     </row>
@@ -5036,11 +5249,11 @@
       <c r="K36" s="14">
         <v>3</v>
       </c>
-      <c r="L36" s="228"/>
-      <c r="M36" s="228"/>
-      <c r="N36" s="228"/>
-      <c r="O36" s="228"/>
-      <c r="P36" s="228"/>
+      <c r="L36" s="230"/>
+      <c r="M36" s="230"/>
+      <c r="N36" s="230"/>
+      <c r="O36" s="230"/>
+      <c r="P36" s="230"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="33">
@@ -5576,10 +5789,10 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="33"/>
-      <c r="B51" s="224" t="s">
+      <c r="B51" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="225"/>
+      <c r="C51" s="227"/>
       <c r="D51" s="4">
         <f>+SUM(D52:D62)</f>
         <v>945</v>
@@ -6176,7 +6389,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="43.2">
-      <c r="A4" s="253">
+      <c r="A4" s="255">
         <v>1</v>
       </c>
       <c r="B4" s="200" t="s">
@@ -6203,7 +6416,7 @@
       <c r="L4" s="203"/>
     </row>
     <row r="5" spans="1:12" ht="57.6">
-      <c r="A5" s="254"/>
+      <c r="A5" s="256"/>
       <c r="B5" s="204" t="s">
         <v>474</v>
       </c>
@@ -6226,7 +6439,7 @@
       <c r="L5" s="207"/>
     </row>
     <row r="6" spans="1:12" ht="43.2">
-      <c r="A6" s="253">
+      <c r="A6" s="255">
         <v>2</v>
       </c>
       <c r="B6" s="200" t="s">
@@ -6251,7 +6464,7 @@
       <c r="L6" s="203"/>
     </row>
     <row r="7" spans="1:12" ht="31.2" customHeight="1">
-      <c r="A7" s="254"/>
+      <c r="A7" s="256"/>
       <c r="B7" s="204" t="s">
         <v>459</v>
       </c>
@@ -6491,22 +6704,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A1" s="255" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="255" t="s">
+      <c r="A1" s="257" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="257" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="257" t="s">
+      <c r="C1" s="259" t="s">
         <v>308</v>
       </c>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="259"/>
+      <c r="D1" s="260"/>
+      <c r="E1" s="260"/>
+      <c r="F1" s="261"/>
     </row>
     <row r="2" spans="1:6" ht="51" thickBot="1">
-      <c r="A2" s="256"/>
-      <c r="B2" s="256"/>
+      <c r="A2" s="258"/>
+      <c r="B2" s="258"/>
       <c r="C2" s="107" t="s">
         <v>309</v>
       </c>
@@ -6884,10 +7097,10 @@
       <c r="F23" s="110"/>
     </row>
     <row r="24" spans="1:6" ht="17.399999999999999" thickBot="1">
-      <c r="A24" s="257" t="s">
+      <c r="A24" s="259" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="259"/>
+      <c r="B24" s="261"/>
       <c r="C24" s="107">
         <f>SUM(C3,C8,C12,C17,C21)</f>
         <v>60</v>
@@ -6932,20 +7145,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999">
-      <c r="A1" s="247"/>
-      <c r="B1" s="247" t="s">
+      <c r="A1" s="249"/>
+      <c r="B1" s="249" t="s">
         <v>337</v>
       </c>
-      <c r="C1" s="247" t="s">
+      <c r="C1" s="249" t="s">
         <v>308</v>
       </c>
-      <c r="D1" s="247"/>
-      <c r="E1" s="247"/>
-      <c r="F1" s="247"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
     </row>
     <row r="2" spans="1:6" ht="69.599999999999994">
-      <c r="A2" s="247"/>
-      <c r="B2" s="247"/>
+      <c r="A2" s="249"/>
+      <c r="B2" s="249"/>
       <c r="C2" s="116" t="s">
         <v>309</v>
       </c>
@@ -7513,8 +7726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8496,6 +8709,1038 @@
         <v>12</v>
       </c>
       <c r="C37" s="193"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G74"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="103.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="193" t="s">
+        <v>525</v>
+      </c>
+      <c r="B1" s="193">
+        <f>SUM(B2:B4)</f>
+        <v>3</v>
+      </c>
+      <c r="C1" s="193">
+        <f t="shared" ref="C1:D1" si="0">SUM(C2:C4)</f>
+        <v>3</v>
+      </c>
+      <c r="D1" s="193">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E1" s="193"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>528</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="193" t="s">
+        <v>529</v>
+      </c>
+      <c r="B5" s="193">
+        <f>SUM(B6:B8)</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="193">
+        <f t="shared" ref="C5:D5" si="1">SUM(C6:C8)</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="193">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="193"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>532</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="193" t="s">
+        <v>533</v>
+      </c>
+      <c r="B9" s="193">
+        <f>SUM(B10:B14)</f>
+        <v>6</v>
+      </c>
+      <c r="C9" s="193">
+        <f t="shared" ref="C9:D9" si="2">SUM(C10:C14)</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="193">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="193"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>534</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>535</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>536</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>537</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>538</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="193" t="s">
+        <v>539</v>
+      </c>
+      <c r="B15" s="193">
+        <f>SUM(B16:B20)</f>
+        <v>6</v>
+      </c>
+      <c r="C15" s="193">
+        <f t="shared" ref="C15:E15" si="3">SUM(C16:C20)</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="193">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="193">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>540</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>541</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>542</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>543</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>544</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="193" t="s">
+        <v>545</v>
+      </c>
+      <c r="B21" s="193">
+        <f>SUM(B22:B23)</f>
+        <v>6</v>
+      </c>
+      <c r="C21" s="193">
+        <f t="shared" ref="C21:E21" si="4">SUM(C22:C23)</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="193">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="E21" s="193">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>546</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>543</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="193" t="s">
+        <v>547</v>
+      </c>
+      <c r="B24" s="193">
+        <f>SUM(B25:B27)</f>
+        <v>6</v>
+      </c>
+      <c r="C24" s="193">
+        <f t="shared" ref="C24:E24" si="5">SUM(C25:C27)</f>
+        <v>3</v>
+      </c>
+      <c r="D24" s="193">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E24" s="193">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>548</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>549</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>550</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="193" t="s">
+        <v>551</v>
+      </c>
+      <c r="B28" s="193">
+        <f>SUM(B29:B32)</f>
+        <v>6</v>
+      </c>
+      <c r="C28" s="193">
+        <f t="shared" ref="C28:E28" si="6">SUM(C29:C32)</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="193">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E28" s="193">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>552</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>554</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>544</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="193" t="s">
+        <v>555</v>
+      </c>
+      <c r="B33" s="193">
+        <f>SUM(B34:B36)</f>
+        <v>6</v>
+      </c>
+      <c r="C33" s="193">
+        <f t="shared" ref="C33:E33" si="7">SUM(C34:C36)</f>
+        <v>2</v>
+      </c>
+      <c r="D33" s="193">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E33" s="193">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>556</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>557</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>558</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="193" t="s">
+        <v>559</v>
+      </c>
+      <c r="B37" s="193">
+        <f>SUM(B38:B42)</f>
+        <v>6</v>
+      </c>
+      <c r="C37" s="193">
+        <f t="shared" ref="C37:E37" si="8">SUM(C38:C42)</f>
+        <v>2</v>
+      </c>
+      <c r="D37" s="193">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E37" s="193">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>560</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>561</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>562</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>563</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>564</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="193" t="s">
+        <v>565</v>
+      </c>
+      <c r="B43" s="193">
+        <f>SUM(B44:B46)</f>
+        <v>6</v>
+      </c>
+      <c r="C43" s="193">
+        <f t="shared" ref="C43:E43" si="9">SUM(C44:C46)</f>
+        <v>1</v>
+      </c>
+      <c r="D43" s="193">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E43" s="193">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>566</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>567</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>568</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="193" t="s">
+        <v>569</v>
+      </c>
+      <c r="B47" s="193">
+        <f>SUM(B48:B53)</f>
+        <v>6</v>
+      </c>
+      <c r="C47" s="193">
+        <f t="shared" ref="C47:E47" si="10">SUM(C48:C53)</f>
+        <v>1</v>
+      </c>
+      <c r="D47" s="193">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="E47" s="193">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>570</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>571</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>572</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>573</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>574</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>575</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="193" t="s">
+        <v>576</v>
+      </c>
+      <c r="B54" s="193">
+        <f>SUM(B55:B59)</f>
+        <v>6</v>
+      </c>
+      <c r="C54" s="193">
+        <f t="shared" ref="C54:D54" si="11">SUM(C55:C59)</f>
+        <v>2</v>
+      </c>
+      <c r="D54" s="193">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E54" s="193"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>577</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>578</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>579</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>580</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>581</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="193" t="s">
+        <v>582</v>
+      </c>
+      <c r="B60" s="193">
+        <f>SUM(B61:B64)</f>
+        <v>3</v>
+      </c>
+      <c r="C60" s="193">
+        <f t="shared" ref="C60:D60" si="12">SUM(C61:C64)</f>
+        <v>0</v>
+      </c>
+      <c r="D60" s="193">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="E60" s="193"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>583</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>584</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>585</v>
+      </c>
+      <c r="B63">
+        <v>0.5</v>
+      </c>
+      <c r="D63">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>586</v>
+      </c>
+      <c r="B64">
+        <v>0.5</v>
+      </c>
+      <c r="D64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="193" customFormat="1">
+      <c r="A65" s="193" t="s">
+        <v>588</v>
+      </c>
+      <c r="B65" s="193">
+        <v>15</v>
+      </c>
+      <c r="D65" s="193">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="193" customFormat="1">
+      <c r="A66" s="193" t="s">
+        <v>587</v>
+      </c>
+      <c r="B66" s="193">
+        <v>6</v>
+      </c>
+      <c r="C66" s="193">
+        <v>1</v>
+      </c>
+      <c r="D66" s="193">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="B67">
+        <f>SUM(B1:B66)/2+(B65+B66)/2</f>
+        <v>90</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:E67" si="13">SUM(C1:C66)/2+(C65+C66)/2</f>
+        <v>24</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="13"/>
+        <v>62</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18">
+      <c r="A72" s="213"/>
+      <c r="B72" s="214"/>
+      <c r="C72" s="214"/>
+      <c r="D72" s="214"/>
+      <c r="E72" s="214"/>
+      <c r="F72" s="213"/>
+      <c r="G72" s="213"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="213"/>
+      <c r="B73" s="213"/>
+      <c r="C73" s="213"/>
+      <c r="D73" s="213"/>
+      <c r="E73" s="213"/>
+      <c r="F73" s="213"/>
+      <c r="G73" s="213"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="213"/>
+      <c r="B74" s="213"/>
+      <c r="C74" s="213"/>
+      <c r="D74" s="213"/>
+      <c r="E74" s="213"/>
+      <c r="F74" s="213"/>
+      <c r="G74" s="213"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="51.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B1">
+        <v>6</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>591</v>
+      </c>
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>593</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8530,59 +9775,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="222" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="221" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221" t="s">
+      <c r="C3" s="223"/>
+      <c r="D3" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="222" t="s">
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="222" t="s">
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="224" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="221"/>
+      <c r="A4" s="223"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -8625,7 +9870,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="222"/>
+      <c r="P4" s="224"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -8658,10 +9903,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="213" t="s">
+      <c r="B6" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -8996,10 +10241,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="215" t="s">
+      <c r="B13" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="216"/>
+      <c r="C13" s="218"/>
       <c r="D13" s="18">
         <f>+D14+D29</f>
         <v>2475</v>
@@ -9022,10 +10267,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8"/>
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="218"/>
+      <c r="C14" s="220"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D28)</f>
         <v>645</v>
@@ -9751,10 +10996,10 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="8"/>
-      <c r="B29" s="219" t="s">
+      <c r="B29" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="219"/>
+      <c r="C29" s="221"/>
       <c r="D29" s="22">
         <f>+SUM(D30:D46)</f>
         <v>1830</v>
@@ -10629,10 +11874,10 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="33"/>
-      <c r="B47" s="224" t="s">
+      <c r="B47" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="225"/>
+      <c r="C47" s="227"/>
       <c r="D47" s="4">
         <f>+SUM(D48:D55)</f>
         <v>855</v>
@@ -11122,59 +12367,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" ht="17.399999999999999">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="222" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
       <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="221" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221" t="s">
+      <c r="C3" s="223"/>
+      <c r="D3" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="222" t="s">
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="222" t="s">
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="224" t="s">
         <v>5</v>
       </c>
       <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" ht="27.6">
-      <c r="A4" s="221"/>
+      <c r="A4" s="223"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -11217,7 +12462,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="222"/>
+      <c r="P4" s="224"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="4"/>
@@ -11249,10 +12494,10 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="4"/>
-      <c r="B6" s="213" t="s">
+      <c r="B6" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -11587,10 +12832,10 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="21"/>
-      <c r="B13" s="215" t="s">
+      <c r="B13" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="216"/>
+      <c r="C13" s="218"/>
       <c r="D13" s="18">
         <f>+D14+D26</f>
         <v>3325</v>
@@ -11613,10 +12858,10 @@
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="8"/>
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="218"/>
+      <c r="C14" s="220"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D25)</f>
         <v>660</v>
@@ -12181,10 +13426,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="8"/>
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="219"/>
+      <c r="C26" s="221"/>
       <c r="D26" s="22">
         <f>+SUM(D27:D49)</f>
         <v>2665</v>
@@ -13175,10 +14420,10 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="33"/>
-      <c r="B50" s="224" t="s">
+      <c r="B50" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="225"/>
+      <c r="C50" s="227"/>
       <c r="D50" s="4">
         <f>+SUM(D51:D61)</f>
         <v>900</v>
@@ -13857,59 +15102,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="222" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="221" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221" t="s">
+      <c r="C3" s="223"/>
+      <c r="D3" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="222" t="s">
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="222" t="s">
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="224" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="221"/>
+      <c r="A4" s="223"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -13952,7 +15197,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="222"/>
+      <c r="P4" s="224"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -13985,10 +15230,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="213" t="s">
+      <c r="B6" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -14323,10 +15568,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="215" t="s">
+      <c r="B13" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="216"/>
+      <c r="C13" s="218"/>
       <c r="D13" s="18">
         <f>+D14+D33</f>
         <v>2520</v>
@@ -14349,10 +15594,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8"/>
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="218"/>
+      <c r="C14" s="220"/>
       <c r="D14" s="22">
         <f>+SUM(D15:D32)</f>
         <v>445</v>
@@ -15099,10 +16344,10 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="8"/>
-      <c r="B33" s="219" t="s">
+      <c r="B33" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="219"/>
+      <c r="C33" s="221"/>
       <c r="D33" s="22">
         <f>+SUM(D34:D50)</f>
         <v>2075</v>
@@ -15763,10 +17008,10 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="33"/>
-      <c r="B51" s="224" t="s">
+      <c r="B51" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="225"/>
+      <c r="C51" s="227"/>
       <c r="D51" s="4">
         <f>+SUM(D52:D58)</f>
         <v>780</v>
@@ -16135,59 +17380,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="17.399999999999999">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="222" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="221" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221" t="s">
+      <c r="C3" s="223"/>
+      <c r="D3" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="222" t="s">
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="222" t="s">
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="224" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="221"/>
+      <c r="A4" s="223"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -16230,7 +17475,7 @@
       <c r="O4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="222"/>
+      <c r="P4" s="224"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -16263,10 +17508,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="4"/>
-      <c r="B6" s="213" t="s">
+      <c r="B6" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="5">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -16601,8 +17846,8 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="229"/>
-      <c r="C13" s="230"/>
+      <c r="B13" s="231"/>
+      <c r="C13" s="232"/>
       <c r="D13" s="18"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -16619,10 +17864,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="21"/>
-      <c r="B14" s="215" t="s">
+      <c r="B14" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="216"/>
+      <c r="C14" s="218"/>
       <c r="D14" s="18">
         <f>+D15+D26</f>
         <v>2460</v>
@@ -16645,10 +17890,10 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="8"/>
-      <c r="B15" s="217" t="s">
+      <c r="B15" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="218"/>
+      <c r="C15" s="220"/>
       <c r="D15" s="22">
         <f>+SUM(D16:D25)</f>
         <v>810</v>
@@ -17191,10 +18436,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="8"/>
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="219"/>
+      <c r="C26" s="221"/>
       <c r="D26" s="22">
         <f>+SUM(D27:D39)</f>
         <v>1650</v>
@@ -17883,10 +19128,10 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="33"/>
-      <c r="B40" s="224" t="s">
+      <c r="B40" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="225"/>
+      <c r="C40" s="227"/>
       <c r="D40" s="4">
         <f>+SUM(D41:D51)</f>
         <v>1230</v>
@@ -18520,59 +19765,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="23.25" customHeight="1">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="222" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
       <c r="AE2" s="2"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="221" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="223" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="221"/>
-      <c r="D3" s="221" t="s">
+      <c r="C3" s="223"/>
+      <c r="D3" s="223" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="221"/>
-      <c r="F3" s="221"/>
-      <c r="G3" s="221"/>
-      <c r="H3" s="222" t="s">
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="222"/>
-      <c r="J3" s="222"/>
-      <c r="K3" s="222"/>
-      <c r="L3" s="223" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="223"/>
-      <c r="N3" s="223"/>
-      <c r="O3" s="223"/>
-      <c r="P3" s="222" t="s">
+      <c r="M3" s="225"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="224" t="s">
         <v>5</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
     <row r="4" spans="1:31" ht="27.6">
-      <c r="A4" s="221"/>
+      <c r="A4" s="223"/>
       <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
@@ -18615,7 +19860,7 @@
       <c r="O4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="222"/>
+      <c r="P4" s="224"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="84"/>
@@ -18648,10 +19893,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="84"/>
-      <c r="B6" s="213" t="s">
+      <c r="B6" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="85">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -18992,8 +20237,8 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="21"/>
-      <c r="B13" s="229"/>
-      <c r="C13" s="230"/>
+      <c r="B13" s="231"/>
+      <c r="C13" s="232"/>
       <c r="D13" s="18"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -19010,10 +20255,10 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="21"/>
-      <c r="B14" s="215" t="s">
+      <c r="B14" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="216"/>
+      <c r="C14" s="218"/>
       <c r="D14" s="18">
         <f>+D15+D26</f>
         <v>2510</v>
@@ -19036,10 +20281,10 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="8"/>
-      <c r="B15" s="217" t="s">
+      <c r="B15" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="218"/>
+      <c r="C15" s="220"/>
       <c r="D15" s="22">
         <f>+SUM(D16:D25)</f>
         <v>860</v>
@@ -19592,10 +20837,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="8"/>
-      <c r="B26" s="219" t="s">
+      <c r="B26" s="221" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="219"/>
+      <c r="C26" s="221"/>
       <c r="D26" s="22">
         <f>+SUM(D27:D38)</f>
         <v>1650</v>
@@ -20254,10 +21499,10 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="33"/>
-      <c r="B39" s="224" t="s">
+      <c r="B39" s="226" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="225"/>
+      <c r="C39" s="227"/>
       <c r="D39" s="84">
         <f>+SUM(D41:D48)</f>
         <v>787</v>
@@ -20686,8 +21931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE47"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:G27"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.25" customHeight="1"/>
@@ -20711,86 +21956,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="34.5" customHeight="1">
-      <c r="A1" s="252" t="s">
+      <c r="A1" s="254" t="s">
         <v>417</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
+      <c r="G1" s="254"/>
     </row>
     <row r="2" spans="1:31" ht="20.25" hidden="1" customHeight="1">
-      <c r="A2" s="249" t="s">
+      <c r="A2" s="251" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249"/>
-      <c r="F2" s="249"/>
-      <c r="G2" s="249"/>
-      <c r="H2" s="249"/>
-      <c r="I2" s="249"/>
-      <c r="J2" s="249"/>
-      <c r="K2" s="249"/>
-      <c r="L2" s="249"/>
-      <c r="M2" s="249"/>
-      <c r="N2" s="249"/>
-      <c r="O2" s="249"/>
-      <c r="P2" s="249"/>
+      <c r="B2" s="251"/>
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="251"/>
+      <c r="J2" s="251"/>
+      <c r="K2" s="251"/>
+      <c r="L2" s="251"/>
+      <c r="M2" s="251"/>
+      <c r="N2" s="251"/>
+      <c r="O2" s="251"/>
+      <c r="P2" s="251"/>
       <c r="AE2" s="146"/>
     </row>
     <row r="3" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="249" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="233" t="s">
+      <c r="B3" s="235" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="234"/>
-      <c r="D3" s="248" t="s">
+      <c r="C3" s="236"/>
+      <c r="D3" s="250" t="s">
         <v>421</v>
       </c>
-      <c r="E3" s="248"/>
-      <c r="F3" s="248"/>
-      <c r="G3" s="248"/>
-      <c r="H3" s="243" t="s">
+      <c r="E3" s="250"/>
+      <c r="F3" s="250"/>
+      <c r="G3" s="250"/>
+      <c r="H3" s="245" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="248"/>
-      <c r="J3" s="248"/>
-      <c r="K3" s="248"/>
-      <c r="L3" s="249" t="s">
+      <c r="I3" s="250"/>
+      <c r="J3" s="250"/>
+      <c r="K3" s="250"/>
+      <c r="L3" s="251" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="249"/>
-      <c r="N3" s="249"/>
-      <c r="O3" s="249"/>
-      <c r="P3" s="241" t="s">
+      <c r="M3" s="251"/>
+      <c r="N3" s="251"/>
+      <c r="O3" s="251"/>
+      <c r="P3" s="243" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="250" t="s">
+      <c r="Q3" s="252" t="s">
         <v>424</v>
       </c>
-      <c r="R3" s="239" t="s">
+      <c r="R3" s="241" t="s">
         <v>427</v>
       </c>
       <c r="AE3" s="146"/>
     </row>
     <row r="4" spans="1:31" ht="20.25" customHeight="1">
-      <c r="A4" s="247"/>
-      <c r="B4" s="235"/>
-      <c r="C4" s="236"/>
-      <c r="D4" s="239" t="s">
+      <c r="A4" s="249"/>
+      <c r="B4" s="237"/>
+      <c r="C4" s="238"/>
+      <c r="D4" s="241" t="s">
         <v>420</v>
       </c>
-      <c r="E4" s="241" t="s">
+      <c r="E4" s="243" t="s">
         <v>422</v>
       </c>
-      <c r="F4" s="242"/>
-      <c r="G4" s="243"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="245"/>
       <c r="H4" s="167"/>
       <c r="I4" s="132"/>
       <c r="J4" s="132"/>
@@ -20799,16 +22044,16 @@
       <c r="M4" s="134"/>
       <c r="N4" s="134"/>
       <c r="O4" s="134"/>
-      <c r="P4" s="241"/>
-      <c r="Q4" s="251"/>
-      <c r="R4" s="240"/>
+      <c r="P4" s="243"/>
+      <c r="Q4" s="253"/>
+      <c r="R4" s="242"/>
       <c r="AE4" s="146"/>
     </row>
     <row r="5" spans="1:31" ht="44.25" customHeight="1">
-      <c r="A5" s="247"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="238"/>
-      <c r="D5" s="240"/>
+      <c r="A5" s="249"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="240"/>
+      <c r="D5" s="242"/>
       <c r="E5" s="134" t="s">
         <v>8</v>
       </c>
@@ -20842,7 +22087,7 @@
       <c r="O5" s="134" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="241"/>
+      <c r="P5" s="243"/>
       <c r="Q5" s="148"/>
       <c r="R5" s="148"/>
     </row>
@@ -20850,10 +22095,10 @@
       <c r="A6" s="132" t="s">
         <v>311</v>
       </c>
-      <c r="B6" s="244" t="s">
+      <c r="B6" s="246" t="s">
         <v>412</v>
       </c>
-      <c r="C6" s="244"/>
+      <c r="C6" s="246"/>
       <c r="D6" s="132">
         <f>+SUM(D7:D12)</f>
         <v>450</v>
@@ -21243,10 +22488,10 @@
       <c r="A13" s="132" t="s">
         <v>317</v>
       </c>
-      <c r="B13" s="245" t="s">
+      <c r="B13" s="247" t="s">
         <v>413</v>
       </c>
-      <c r="C13" s="245"/>
+      <c r="C13" s="247"/>
       <c r="D13" s="134">
         <f>+D14+D25</f>
         <v>3300</v>
@@ -21306,10 +22551,10 @@
       <c r="A14" s="132" t="s">
         <v>415</v>
       </c>
-      <c r="B14" s="244" t="s">
+      <c r="B14" s="246" t="s">
         <v>414</v>
       </c>
-      <c r="C14" s="246"/>
+      <c r="C14" s="248"/>
       <c r="D14" s="149">
         <f>+SUM(D15:D24)</f>
         <v>860</v>
@@ -21915,10 +23160,10 @@
       <c r="A25" s="132" t="s">
         <v>416</v>
       </c>
-      <c r="B25" s="244" t="s">
+      <c r="B25" s="246" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="244"/>
+      <c r="C25" s="246"/>
       <c r="D25" s="149">
         <f>+SUM(D26:D46)</f>
         <v>2440</v>
@@ -23048,10 +24293,10 @@
       </c>
     </row>
     <row r="47" spans="1:18" ht="20.25" customHeight="1">
-      <c r="A47" s="231" t="s">
+      <c r="A47" s="233" t="s">
         <v>418</v>
       </c>
-      <c r="B47" s="232"/>
+      <c r="B47" s="234"/>
       <c r="C47" s="148"/>
       <c r="D47" s="128">
         <f>SUM(D6,D13)</f>

</xml_diff>